<commit_message>
Compute oob score; Better control over hog params
</commit_message>
<xml_diff>
--- a/resultats/random_forest_gridsearch.xlsx
+++ b/resultats/random_forest_gridsearch.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/resultats/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="860" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="SIFT" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="CIFAR10-HOG" sheetId="3" r:id="rId1"/>
+    <sheet name="MNIST-SIFT" sheetId="1" r:id="rId2"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch_accuracy_test" localSheetId="1">Feuil2!$F$9:$H$11</definedName>
-    <definedName name="gridsearch_accuracy_test" localSheetId="0">SIFT!$P$4:$S$9</definedName>
-    <definedName name="gridsearch_accuracy_test_1" localSheetId="0">SIFT!$L$9:$P$12</definedName>
-    <definedName name="gridsearch_accuracy_test_2" localSheetId="0">SIFT!$C$21:$D$23</definedName>
-    <definedName name="gridsearch_accuracy_train" localSheetId="1">Feuil2!$B$9:$D$11</definedName>
-    <definedName name="gridsearch_accuracy_train" localSheetId="0">SIFT!$G$4:$J$9</definedName>
+    <definedName name="gridsearch_accuracy_test" localSheetId="2">Feuil2!$F$9:$H$11</definedName>
+    <definedName name="gridsearch_accuracy_test" localSheetId="1">'MNIST-SIFT'!$P$4:$S$9</definedName>
+    <definedName name="gridsearch_accuracy_test_1" localSheetId="1">'MNIST-SIFT'!$L$9:$P$12</definedName>
+    <definedName name="gridsearch_accuracy_test_2" localSheetId="1">'MNIST-SIFT'!$C$21:$D$23</definedName>
+    <definedName name="gridsearch_accuracy_train" localSheetId="2">Feuil2!$B$9:$D$11</definedName>
+    <definedName name="gridsearch_accuracy_train" localSheetId="1">'MNIST-SIFT'!$G$4:$J$9</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Maximum features to consider</t>
   </si>
@@ -134,11 +135,21 @@
   <si>
     <t>6 words</t>
   </si>
+  <si>
+    <t>Max. features to consider</t>
+  </si>
+  <si>
+    <t>Num. estimators</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -177,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -305,12 +316,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -360,9 +386,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -380,14 +415,14 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -405,7 +440,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,7 +448,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,11 +456,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,10 +726,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.83203125" customWidth="1"/>
+    <col min="11" max="17" width="8.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C1" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C2" s="49">
+        <v>8</v>
+      </c>
+      <c r="D2" s="49">
+        <v>10</v>
+      </c>
+      <c r="E2" s="49">
+        <v>11</v>
+      </c>
+      <c r="F2" s="49">
+        <v>12</v>
+      </c>
+      <c r="G2" s="49">
+        <v>16</v>
+      </c>
+      <c r="H2" s="49">
+        <v>32</v>
+      </c>
+      <c r="I2" s="49">
+        <v>64</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="49">
+        <v>8</v>
+      </c>
+      <c r="L2" s="49">
+        <v>10</v>
+      </c>
+      <c r="M2" s="49">
+        <v>11</v>
+      </c>
+      <c r="N2" s="49">
+        <v>12</v>
+      </c>
+      <c r="O2" s="49">
+        <v>16</v>
+      </c>
+      <c r="P2" s="49">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="49">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="49">
+        <v>10</v>
+      </c>
+      <c r="C3" s="47">
+        <v>0.99451999999999896</v>
+      </c>
+      <c r="D3" s="47">
+        <v>0.994779999999999</v>
+      </c>
+      <c r="E3" s="47">
+        <v>0.99448000000000003</v>
+      </c>
+      <c r="F3" s="47">
+        <v>0.99439999999999895</v>
+      </c>
+      <c r="G3" s="47">
+        <v>0.99448000000000003</v>
+      </c>
+      <c r="H3" s="47">
+        <v>0.99431999999999898</v>
+      </c>
+      <c r="I3" s="47">
+        <v>0.99409999999999898</v>
+      </c>
+      <c r="K3" s="46">
+        <v>0.31609999999999899</v>
+      </c>
+      <c r="L3" s="46">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M3" s="46">
+        <v>0.3261</v>
+      </c>
+      <c r="N3" s="46">
+        <v>0.32190000000000002</v>
+      </c>
+      <c r="O3" s="46">
+        <v>0.32750000000000001</v>
+      </c>
+      <c r="P3" s="46">
+        <v>0.34</v>
+      </c>
+      <c r="Q3" s="46">
+        <v>0.34589999999999899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="50"/>
+      <c r="B4" s="49">
+        <v>100</v>
+      </c>
+      <c r="C4" s="47">
+        <v>1</v>
+      </c>
+      <c r="D4" s="47">
+        <v>1</v>
+      </c>
+      <c r="E4" s="47">
+        <v>1</v>
+      </c>
+      <c r="F4" s="47">
+        <v>1</v>
+      </c>
+      <c r="G4" s="47">
+        <v>1</v>
+      </c>
+      <c r="H4" s="47">
+        <v>1</v>
+      </c>
+      <c r="I4" s="47">
+        <v>1</v>
+      </c>
+      <c r="K4" s="46">
+        <v>0.47599999999999898</v>
+      </c>
+      <c r="L4" s="46">
+        <v>0.47449999999999898</v>
+      </c>
+      <c r="M4" s="46">
+        <v>0.4773</v>
+      </c>
+      <c r="N4" s="46">
+        <v>0.472299999999999</v>
+      </c>
+      <c r="O4" s="46">
+        <v>0.47389999999999899</v>
+      </c>
+      <c r="P4" s="46">
+        <v>0.47239999999999899</v>
+      </c>
+      <c r="Q4" s="46">
+        <v>0.47610000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="50"/>
+      <c r="B5" s="49">
+        <v>200</v>
+      </c>
+      <c r="C5" s="47">
+        <v>1</v>
+      </c>
+      <c r="D5" s="47">
+        <v>1</v>
+      </c>
+      <c r="E5" s="47">
+        <v>1</v>
+      </c>
+      <c r="F5" s="47">
+        <v>1</v>
+      </c>
+      <c r="G5" s="47">
+        <v>1</v>
+      </c>
+      <c r="H5" s="47">
+        <v>1</v>
+      </c>
+      <c r="I5" s="47">
+        <v>1</v>
+      </c>
+      <c r="K5" s="46">
+        <v>0.49569999999999897</v>
+      </c>
+      <c r="L5" s="46">
+        <v>0.49840000000000001</v>
+      </c>
+      <c r="M5" s="46">
+        <v>0.49890000000000001</v>
+      </c>
+      <c r="N5" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="46">
+        <v>0.493999999999999</v>
+      </c>
+      <c r="P5" s="46">
+        <v>0.49120000000000003</v>
+      </c>
+      <c r="Q5" s="46">
+        <v>0.48930000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="50"/>
+      <c r="B6" s="49">
+        <v>500</v>
+      </c>
+      <c r="C6" s="47">
+        <v>1</v>
+      </c>
+      <c r="D6" s="47">
+        <v>1</v>
+      </c>
+      <c r="E6" s="47">
+        <v>1</v>
+      </c>
+      <c r="F6" s="47">
+        <v>1</v>
+      </c>
+      <c r="G6" s="47">
+        <v>1</v>
+      </c>
+      <c r="H6" s="47">
+        <v>1</v>
+      </c>
+      <c r="I6" s="47">
+        <v>1</v>
+      </c>
+      <c r="K6" s="46">
+        <v>0.51419999999999899</v>
+      </c>
+      <c r="L6" s="46">
+        <v>0.507099999999999</v>
+      </c>
+      <c r="M6" s="46">
+        <v>0.50949999999999895</v>
+      </c>
+      <c r="N6" s="46">
+        <v>0.50639999999999896</v>
+      </c>
+      <c r="O6" s="46">
+        <v>0.50880000000000003</v>
+      </c>
+      <c r="P6" s="46">
+        <v>0.49990000000000001</v>
+      </c>
+      <c r="Q6" s="46">
+        <v>0.50039999999999896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="50"/>
+      <c r="B7" s="49">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="47">
+        <v>1</v>
+      </c>
+      <c r="D7" s="47">
+        <v>1</v>
+      </c>
+      <c r="E7" s="47">
+        <v>1</v>
+      </c>
+      <c r="F7" s="47">
+        <v>1</v>
+      </c>
+      <c r="G7" s="47">
+        <v>1</v>
+      </c>
+      <c r="H7" s="47">
+        <v>1</v>
+      </c>
+      <c r="I7" s="47">
+        <v>1</v>
+      </c>
+      <c r="K7" s="46">
+        <v>0.51590000000000003</v>
+      </c>
+      <c r="L7" s="46">
+        <v>0.51180000000000003</v>
+      </c>
+      <c r="M7" s="46">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="N7" s="46">
+        <v>0.51229999999999898</v>
+      </c>
+      <c r="O7" s="46">
+        <v>0.51090000000000002</v>
+      </c>
+      <c r="P7" s="46">
+        <v>0.50449999999999895</v>
+      </c>
+      <c r="Q7" s="46">
+        <v>0.50519999999999898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="50"/>
+      <c r="B8" s="49">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="47">
+        <v>1</v>
+      </c>
+      <c r="D8" s="47">
+        <v>1</v>
+      </c>
+      <c r="E8" s="47">
+        <v>1</v>
+      </c>
+      <c r="F8" s="47">
+        <v>1</v>
+      </c>
+      <c r="G8" s="47">
+        <v>1</v>
+      </c>
+      <c r="H8" s="47">
+        <v>1</v>
+      </c>
+      <c r="I8" s="47">
+        <v>1</v>
+      </c>
+      <c r="K8" s="46">
+        <v>0.51590000000000003</v>
+      </c>
+      <c r="L8" s="46">
+        <v>0.51559999999999895</v>
+      </c>
+      <c r="M8" s="46">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="N8" s="46">
+        <v>0.51649999999999896</v>
+      </c>
+      <c r="O8" s="46">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="P8" s="46">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="Q8" s="46">
+        <v>0.50929999999999898</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="K1:Q1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="K3:Q8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,48 +1138,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="45"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="40"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C3" s="23">
@@ -804,7 +1233,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -845,7 +1274,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5">
         <v>2</v>
       </c>
@@ -884,7 +1313,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -923,7 +1352,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -962,7 +1391,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8">
         <v>20</v>
       </c>
@@ -1001,17 +1430,17 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="42">
         <v>0.999966666666666</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="8">
         <v>0.999966666666666</v>
       </c>
@@ -1048,15 +1477,15 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="11"/>
@@ -1081,15 +1510,15 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11">
         <v>200</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="11"/>
@@ -1114,15 +1543,15 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12">
         <v>1000</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
@@ -1179,20 +1608,20 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="41"/>
+      <c r="C16" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
       <c r="K16" s="27"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -1204,8 +1633,8 @@
       <c r="S16" s="28"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="24" t="s">
         <v>13</v>
       </c>
@@ -1237,7 +1666,7 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="29">
@@ -1262,7 +1691,7 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="29">
         <v>100</v>
       </c>
@@ -1295,7 +1724,7 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="30">
         <v>200</v>
       </c>
@@ -1322,7 +1751,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="30">
         <v>500</v>
       </c>
@@ -1345,7 +1774,7 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="31">
         <v>1000</v>
       </c>
@@ -1364,7 +1793,7 @@
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="31">
         <v>2000</v>
       </c>
@@ -1383,7 +1812,7 @@
       <c r="K23" s="33"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="34"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1396,7 +1825,7 @@
       <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="31"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1549,7 +1978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>

</xml_diff>

<commit_message>
New features and parameters
</commit_message>
<xml_diff>
--- a/resultats/random_forest_gridsearch.xlsx
+++ b/resultats/random_forest_gridsearch.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR10-HOG" sheetId="3" r:id="rId1"/>
-    <sheet name="MNIST-SIFT" sheetId="1" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
+    <sheet name="CIFAR10-DSHOG" sheetId="4" r:id="rId2"/>
+    <sheet name="MNIST-SIFT" sheetId="1" r:id="rId3"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch_accuracy_test" localSheetId="2">Feuil2!$F$9:$H$11</definedName>
-    <definedName name="gridsearch_accuracy_test" localSheetId="1">'MNIST-SIFT'!$P$4:$S$9</definedName>
-    <definedName name="gridsearch_accuracy_test_1" localSheetId="1">'MNIST-SIFT'!$L$9:$P$12</definedName>
-    <definedName name="gridsearch_accuracy_test_2" localSheetId="1">'MNIST-SIFT'!$C$21:$D$23</definedName>
-    <definedName name="gridsearch_accuracy_train" localSheetId="2">Feuil2!$B$9:$D$11</definedName>
-    <definedName name="gridsearch_accuracy_train" localSheetId="1">'MNIST-SIFT'!$G$4:$J$9</definedName>
+    <definedName name="gridsearch_accuracy_test" localSheetId="3">Feuil2!$F$9:$H$11</definedName>
+    <definedName name="gridsearch_accuracy_test" localSheetId="2">'MNIST-SIFT'!$P$4:$S$9</definedName>
+    <definedName name="gridsearch_accuracy_test_1" localSheetId="2">'MNIST-SIFT'!$L$9:$P$12</definedName>
+    <definedName name="gridsearch_accuracy_test_2" localSheetId="2">'MNIST-SIFT'!$C$21:$D$23</definedName>
+    <definedName name="gridsearch_accuracy_train" localSheetId="3">Feuil2!$B$9:$D$11</definedName>
+    <definedName name="gridsearch_accuracy_train" localSheetId="2">'MNIST-SIFT'!$G$4:$J$9</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Maximum features to consider</t>
   </si>
@@ -141,14 +142,20 @@
   <si>
     <t>Num. estimators</t>
   </si>
+  <si>
+    <t>Max. features</t>
+  </si>
+  <si>
+    <t>Min samples split</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -336,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -385,6 +392,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,15 +431,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +460,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,7 +468,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,11 +476,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,358 +761,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C2" s="49">
+      <c r="C2" s="38">
         <v>8</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="38">
         <v>10</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="38">
         <v>11</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="38">
         <v>12</v>
       </c>
-      <c r="G2" s="49">
+      <c r="G2" s="38">
         <v>16</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="38">
         <v>32</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="38">
         <v>64</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="49">
+      <c r="K2" s="38">
         <v>8</v>
       </c>
-      <c r="L2" s="49">
+      <c r="L2" s="38">
         <v>10</v>
       </c>
-      <c r="M2" s="49">
+      <c r="M2" s="38">
         <v>11</v>
       </c>
-      <c r="N2" s="49">
+      <c r="N2" s="38">
         <v>12</v>
       </c>
-      <c r="O2" s="49">
+      <c r="O2" s="38">
         <v>16</v>
       </c>
-      <c r="P2" s="49">
+      <c r="P2" s="38">
         <v>32</v>
       </c>
-      <c r="Q2" s="49">
+      <c r="Q2" s="38">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="38">
         <v>10</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="37">
         <v>0.99451999999999896</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="37">
         <v>0.994779999999999</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="37">
         <v>0.99448000000000003</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="37">
         <v>0.99439999999999895</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="37">
         <v>0.99448000000000003</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="37">
         <v>0.99431999999999898</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="37">
         <v>0.99409999999999898</v>
       </c>
-      <c r="K3" s="46">
+      <c r="K3" s="36">
         <v>0.31609999999999899</v>
       </c>
-      <c r="L3" s="46">
+      <c r="L3" s="36">
         <v>0.32200000000000001</v>
       </c>
-      <c r="M3" s="46">
+      <c r="M3" s="36">
         <v>0.3261</v>
       </c>
-      <c r="N3" s="46">
+      <c r="N3" s="36">
         <v>0.32190000000000002</v>
       </c>
-      <c r="O3" s="46">
+      <c r="O3" s="36">
         <v>0.32750000000000001</v>
       </c>
-      <c r="P3" s="46">
+      <c r="P3" s="36">
         <v>0.34</v>
       </c>
-      <c r="Q3" s="46">
+      <c r="Q3" s="36">
         <v>0.34589999999999899</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
-      <c r="B4" s="49">
+      <c r="A4" s="40"/>
+      <c r="B4" s="38">
         <v>100</v>
       </c>
-      <c r="C4" s="47">
-        <v>1</v>
-      </c>
-      <c r="D4" s="47">
-        <v>1</v>
-      </c>
-      <c r="E4" s="47">
-        <v>1</v>
-      </c>
-      <c r="F4" s="47">
-        <v>1</v>
-      </c>
-      <c r="G4" s="47">
-        <v>1</v>
-      </c>
-      <c r="H4" s="47">
-        <v>1</v>
-      </c>
-      <c r="I4" s="47">
-        <v>1</v>
-      </c>
-      <c r="K4" s="46">
+      <c r="C4" s="37">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37">
+        <v>1</v>
+      </c>
+      <c r="E4" s="37">
+        <v>1</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1</v>
+      </c>
+      <c r="G4" s="37">
+        <v>1</v>
+      </c>
+      <c r="H4" s="37">
+        <v>1</v>
+      </c>
+      <c r="I4" s="37">
+        <v>1</v>
+      </c>
+      <c r="K4" s="36">
         <v>0.47599999999999898</v>
       </c>
-      <c r="L4" s="46">
+      <c r="L4" s="36">
         <v>0.47449999999999898</v>
       </c>
-      <c r="M4" s="46">
+      <c r="M4" s="36">
         <v>0.4773</v>
       </c>
-      <c r="N4" s="46">
+      <c r="N4" s="36">
         <v>0.472299999999999</v>
       </c>
-      <c r="O4" s="46">
+      <c r="O4" s="36">
         <v>0.47389999999999899</v>
       </c>
-      <c r="P4" s="46">
+      <c r="P4" s="36">
         <v>0.47239999999999899</v>
       </c>
-      <c r="Q4" s="46">
+      <c r="Q4" s="36">
         <v>0.47610000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="50"/>
-      <c r="B5" s="49">
+      <c r="A5" s="40"/>
+      <c r="B5" s="38">
         <v>200</v>
       </c>
-      <c r="C5" s="47">
-        <v>1</v>
-      </c>
-      <c r="D5" s="47">
-        <v>1</v>
-      </c>
-      <c r="E5" s="47">
-        <v>1</v>
-      </c>
-      <c r="F5" s="47">
-        <v>1</v>
-      </c>
-      <c r="G5" s="47">
-        <v>1</v>
-      </c>
-      <c r="H5" s="47">
-        <v>1</v>
-      </c>
-      <c r="I5" s="47">
-        <v>1</v>
-      </c>
-      <c r="K5" s="46">
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37">
+        <v>1</v>
+      </c>
+      <c r="E5" s="37">
+        <v>1</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="G5" s="37">
+        <v>1</v>
+      </c>
+      <c r="H5" s="37">
+        <v>1</v>
+      </c>
+      <c r="I5" s="37">
+        <v>1</v>
+      </c>
+      <c r="K5" s="36">
         <v>0.49569999999999897</v>
       </c>
-      <c r="L5" s="46">
+      <c r="L5" s="36">
         <v>0.49840000000000001</v>
       </c>
-      <c r="M5" s="46">
+      <c r="M5" s="36">
         <v>0.49890000000000001</v>
       </c>
-      <c r="N5" s="46">
+      <c r="N5" s="36">
         <v>0.5</v>
       </c>
-      <c r="O5" s="46">
+      <c r="O5" s="36">
         <v>0.493999999999999</v>
       </c>
-      <c r="P5" s="46">
+      <c r="P5" s="36">
         <v>0.49120000000000003</v>
       </c>
-      <c r="Q5" s="46">
+      <c r="Q5" s="36">
         <v>0.48930000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="49">
+      <c r="A6" s="40"/>
+      <c r="B6" s="38">
         <v>500</v>
       </c>
-      <c r="C6" s="47">
-        <v>1</v>
-      </c>
-      <c r="D6" s="47">
-        <v>1</v>
-      </c>
-      <c r="E6" s="47">
-        <v>1</v>
-      </c>
-      <c r="F6" s="47">
-        <v>1</v>
-      </c>
-      <c r="G6" s="47">
-        <v>1</v>
-      </c>
-      <c r="H6" s="47">
-        <v>1</v>
-      </c>
-      <c r="I6" s="47">
-        <v>1</v>
-      </c>
-      <c r="K6" s="46">
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37">
+        <v>1</v>
+      </c>
+      <c r="E6" s="37">
+        <v>1</v>
+      </c>
+      <c r="F6" s="37">
+        <v>1</v>
+      </c>
+      <c r="G6" s="37">
+        <v>1</v>
+      </c>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+      <c r="I6" s="37">
+        <v>1</v>
+      </c>
+      <c r="K6" s="36">
         <v>0.51419999999999899</v>
       </c>
-      <c r="L6" s="46">
+      <c r="L6" s="36">
         <v>0.507099999999999</v>
       </c>
-      <c r="M6" s="46">
+      <c r="M6" s="36">
         <v>0.50949999999999895</v>
       </c>
-      <c r="N6" s="46">
+      <c r="N6" s="36">
         <v>0.50639999999999896</v>
       </c>
-      <c r="O6" s="46">
+      <c r="O6" s="36">
         <v>0.50880000000000003</v>
       </c>
-      <c r="P6" s="46">
+      <c r="P6" s="36">
         <v>0.49990000000000001</v>
       </c>
-      <c r="Q6" s="46">
+      <c r="Q6" s="36">
         <v>0.50039999999999896</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
-      <c r="B7" s="49">
+      <c r="A7" s="40"/>
+      <c r="B7" s="38">
         <v>1000</v>
       </c>
-      <c r="C7" s="47">
-        <v>1</v>
-      </c>
-      <c r="D7" s="47">
-        <v>1</v>
-      </c>
-      <c r="E7" s="47">
-        <v>1</v>
-      </c>
-      <c r="F7" s="47">
-        <v>1</v>
-      </c>
-      <c r="G7" s="47">
-        <v>1</v>
-      </c>
-      <c r="H7" s="47">
-        <v>1</v>
-      </c>
-      <c r="I7" s="47">
-        <v>1</v>
-      </c>
-      <c r="K7" s="46">
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37">
+        <v>1</v>
+      </c>
+      <c r="E7" s="37">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37">
+        <v>1</v>
+      </c>
+      <c r="G7" s="37">
+        <v>1</v>
+      </c>
+      <c r="H7" s="37">
+        <v>1</v>
+      </c>
+      <c r="I7" s="37">
+        <v>1</v>
+      </c>
+      <c r="K7" s="36">
         <v>0.51590000000000003</v>
       </c>
-      <c r="L7" s="46">
+      <c r="L7" s="36">
         <v>0.51180000000000003</v>
       </c>
-      <c r="M7" s="46">
+      <c r="M7" s="36">
         <v>0.51500000000000001</v>
       </c>
-      <c r="N7" s="46">
+      <c r="N7" s="36">
         <v>0.51229999999999898</v>
       </c>
-      <c r="O7" s="46">
+      <c r="O7" s="36">
         <v>0.51090000000000002</v>
       </c>
-      <c r="P7" s="46">
+      <c r="P7" s="36">
         <v>0.50449999999999895</v>
       </c>
-      <c r="Q7" s="46">
+      <c r="Q7" s="36">
         <v>0.50519999999999898</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
-      <c r="B8" s="49">
+      <c r="A8" s="40"/>
+      <c r="B8" s="38">
         <v>2000</v>
       </c>
-      <c r="C8" s="47">
-        <v>1</v>
-      </c>
-      <c r="D8" s="47">
-        <v>1</v>
-      </c>
-      <c r="E8" s="47">
-        <v>1</v>
-      </c>
-      <c r="F8" s="47">
-        <v>1</v>
-      </c>
-      <c r="G8" s="47">
-        <v>1</v>
-      </c>
-      <c r="H8" s="47">
-        <v>1</v>
-      </c>
-      <c r="I8" s="47">
-        <v>1</v>
-      </c>
-      <c r="K8" s="46">
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="37">
+        <v>1</v>
+      </c>
+      <c r="E8" s="37">
+        <v>1</v>
+      </c>
+      <c r="F8" s="37">
+        <v>1</v>
+      </c>
+      <c r="G8" s="37">
+        <v>1</v>
+      </c>
+      <c r="H8" s="37">
+        <v>1</v>
+      </c>
+      <c r="I8" s="37">
+        <v>1</v>
+      </c>
+      <c r="K8" s="36">
         <v>0.51590000000000003</v>
       </c>
-      <c r="L8" s="46">
+      <c r="L8" s="36">
         <v>0.51559999999999895</v>
       </c>
-      <c r="M8" s="46">
+      <c r="M8" s="36">
         <v>0.51570000000000005</v>
       </c>
-      <c r="N8" s="46">
+      <c r="N8" s="36">
         <v>0.51649999999999896</v>
       </c>
-      <c r="O8" s="46">
+      <c r="O8" s="36">
         <v>0.51400000000000001</v>
       </c>
-      <c r="P8" s="46">
+      <c r="P8" s="36">
         <v>0.50800000000000001</v>
       </c>
-      <c r="Q8" s="46">
+      <c r="Q8" s="36">
         <v>0.50929999999999898</v>
       </c>
     </row>
@@ -1103,6 +1123,601 @@
     <mergeCell ref="K1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:Q8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="3" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" customWidth="1"/>
+    <col min="12" max="15" width="8.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C1" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C2" s="51">
+        <v>4</v>
+      </c>
+      <c r="D2" s="51">
+        <v>6</v>
+      </c>
+      <c r="E2" s="51">
+        <v>8</v>
+      </c>
+      <c r="F2" s="51">
+        <v>10</v>
+      </c>
+      <c r="G2" s="51">
+        <v>12</v>
+      </c>
+      <c r="H2" s="51">
+        <v>32</v>
+      </c>
+      <c r="I2" s="51">
+        <v>48</v>
+      </c>
+      <c r="J2" s="57"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="51">
+        <v>4</v>
+      </c>
+      <c r="M2" s="51">
+        <v>6</v>
+      </c>
+      <c r="N2" s="51">
+        <v>8</v>
+      </c>
+      <c r="O2" s="51">
+        <v>10</v>
+      </c>
+      <c r="P2" s="51">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="51">
+        <v>32</v>
+      </c>
+      <c r="R2" s="51">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="38">
+        <v>10</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0.99370000000000003</v>
+      </c>
+      <c r="D3" s="37">
+        <v>0.99331999999999898</v>
+      </c>
+      <c r="E3" s="37">
+        <v>0.99363999999999897</v>
+      </c>
+      <c r="F3" s="37">
+        <v>0.99353999999999898</v>
+      </c>
+      <c r="G3" s="37">
+        <v>0.99316000000000004</v>
+      </c>
+      <c r="H3" s="37">
+        <v>0.99216000000000004</v>
+      </c>
+      <c r="I3" s="37">
+        <v>0.99160000000000004</v>
+      </c>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38">
+        <v>10</v>
+      </c>
+      <c r="L3" s="36">
+        <v>0.40150000000000002</v>
+      </c>
+      <c r="M3" s="36">
+        <v>0.41049999999999898</v>
+      </c>
+      <c r="N3" s="36">
+        <v>0.40949999999999898</v>
+      </c>
+      <c r="O3" s="36">
+        <v>0.41170000000000001</v>
+      </c>
+      <c r="P3" s="36">
+        <v>0.41589999999999899</v>
+      </c>
+      <c r="Q3" s="36">
+        <v>0.42209999999999898</v>
+      </c>
+      <c r="R3" s="36">
+        <v>0.422899999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="40"/>
+      <c r="B4" s="38">
+        <v>100</v>
+      </c>
+      <c r="C4" s="37">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37">
+        <v>1</v>
+      </c>
+      <c r="E4" s="37">
+        <v>1</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1</v>
+      </c>
+      <c r="G4" s="37">
+        <v>1</v>
+      </c>
+      <c r="H4" s="37">
+        <v>1</v>
+      </c>
+      <c r="I4" s="37">
+        <v>1</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38">
+        <v>100</v>
+      </c>
+      <c r="L4" s="36">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="M4" s="36">
+        <v>0.51470000000000005</v>
+      </c>
+      <c r="N4" s="36">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="O4" s="36">
+        <v>0.51839999999999897</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0.51580000000000004</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>0.51659999999999895</v>
+      </c>
+      <c r="R4" s="36">
+        <v>0.50939999999999896</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="40"/>
+      <c r="B5" s="38">
+        <v>300</v>
+      </c>
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37">
+        <v>1</v>
+      </c>
+      <c r="E5" s="37">
+        <v>1</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="G5" s="37">
+        <v>1</v>
+      </c>
+      <c r="H5" s="37">
+        <v>1</v>
+      </c>
+      <c r="I5" s="37">
+        <v>1</v>
+      </c>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38">
+        <v>300</v>
+      </c>
+      <c r="L5" s="36">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="M5" s="36">
+        <v>0.534299999999999</v>
+      </c>
+      <c r="N5" s="36">
+        <v>0.532299999999999</v>
+      </c>
+      <c r="O5" s="36">
+        <v>0.53469999999999895</v>
+      </c>
+      <c r="P5" s="36">
+        <v>0.53149999999999897</v>
+      </c>
+      <c r="Q5" s="36">
+        <v>0.52549999999999897</v>
+      </c>
+      <c r="R5" s="36">
+        <v>0.52139999999999898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="40"/>
+      <c r="B6" s="52">
+        <v>500</v>
+      </c>
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37">
+        <v>1</v>
+      </c>
+      <c r="E6" s="37">
+        <v>1</v>
+      </c>
+      <c r="F6" s="37">
+        <v>1</v>
+      </c>
+      <c r="G6" s="37">
+        <v>1</v>
+      </c>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+      <c r="I6" s="37">
+        <v>1</v>
+      </c>
+      <c r="J6" s="37"/>
+      <c r="K6" s="52">
+        <v>500</v>
+      </c>
+      <c r="L6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="M6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="N6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="O6">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="P6">
+        <v>0.53600000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="40"/>
+      <c r="B7" s="52">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37">
+        <v>1</v>
+      </c>
+      <c r="E7" s="37">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37">
+        <v>1</v>
+      </c>
+      <c r="G7" s="37">
+        <v>1</v>
+      </c>
+      <c r="H7" s="37">
+        <v>1</v>
+      </c>
+      <c r="I7" s="37">
+        <v>1</v>
+      </c>
+      <c r="J7" s="37"/>
+      <c r="K7" s="52">
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="M7">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="N7">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="O7">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="P7">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="40"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C10" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="L10" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C11" s="38">
+        <v>6</v>
+      </c>
+      <c r="D11" s="38">
+        <v>8</v>
+      </c>
+      <c r="E11" s="38">
+        <v>10</v>
+      </c>
+      <c r="F11" s="38">
+        <v>12</v>
+      </c>
+      <c r="L11" s="38">
+        <v>6</v>
+      </c>
+      <c r="M11" s="38">
+        <v>8</v>
+      </c>
+      <c r="N11" s="38">
+        <v>10</v>
+      </c>
+      <c r="O11" s="38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="38">
+        <v>2</v>
+      </c>
+      <c r="C12" s="53">
+        <v>1</v>
+      </c>
+      <c r="D12" s="53">
+        <v>1</v>
+      </c>
+      <c r="E12" s="53">
+        <v>1</v>
+      </c>
+      <c r="F12" s="53">
+        <v>1</v>
+      </c>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="38">
+        <v>2</v>
+      </c>
+      <c r="L12" s="53">
+        <v>0.535299999999999</v>
+      </c>
+      <c r="M12" s="53">
+        <v>0.53469999999999895</v>
+      </c>
+      <c r="N12" s="53">
+        <v>0.53759999999999897</v>
+      </c>
+      <c r="O12" s="53">
+        <v>0.53600000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="55"/>
+      <c r="B13" s="38">
+        <v>4</v>
+      </c>
+      <c r="C13" s="53">
+        <v>1</v>
+      </c>
+      <c r="D13" s="53">
+        <v>1</v>
+      </c>
+      <c r="E13" s="53">
+        <v>1</v>
+      </c>
+      <c r="F13" s="53">
+        <v>1</v>
+      </c>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="38">
+        <v>4</v>
+      </c>
+      <c r="L13" s="53">
+        <v>0.52880000000000005</v>
+      </c>
+      <c r="M13" s="53">
+        <v>0.53469999999999895</v>
+      </c>
+      <c r="N13" s="53">
+        <v>0.53649999999999898</v>
+      </c>
+      <c r="O13" s="53">
+        <v>0.53810000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="55"/>
+      <c r="B14" s="38">
+        <v>8</v>
+      </c>
+      <c r="C14" s="53">
+        <v>0.99882000000000004</v>
+      </c>
+      <c r="D14" s="53">
+        <v>0.99895999999999896</v>
+      </c>
+      <c r="E14" s="53">
+        <v>0.99904000000000004</v>
+      </c>
+      <c r="F14" s="53">
+        <v>0.99914000000000003</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="38">
+        <v>8</v>
+      </c>
+      <c r="L14" s="53">
+        <v>0.52990000000000004</v>
+      </c>
+      <c r="M14" s="53">
+        <v>0.53010000000000002</v>
+      </c>
+      <c r="N14" s="53">
+        <v>0.53210000000000002</v>
+      </c>
+      <c r="O14" s="53">
+        <v>0.53210000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="55"/>
+      <c r="B15" s="38">
+        <v>16</v>
+      </c>
+      <c r="C15" s="53">
+        <v>0.96962000000000004</v>
+      </c>
+      <c r="D15" s="53">
+        <v>0.97206000000000004</v>
+      </c>
+      <c r="E15" s="53">
+        <v>0.97418000000000005</v>
+      </c>
+      <c r="F15" s="53">
+        <v>0.97543999999999897</v>
+      </c>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="38">
+        <v>16</v>
+      </c>
+      <c r="L15" s="53">
+        <v>0.52239999999999898</v>
+      </c>
+      <c r="M15" s="53">
+        <v>0.522199999999999</v>
+      </c>
+      <c r="N15" s="53">
+        <v>0.52539999999999898</v>
+      </c>
+      <c r="O15" s="53">
+        <v>0.52449999999999897</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="L8:R8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:R7">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:O15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1118,7 +1733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
@@ -1138,48 +1753,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="40"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="45"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C3" s="23">
@@ -1233,7 +1848,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -1274,7 +1889,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="42"/>
       <c r="B5">
         <v>2</v>
       </c>
@@ -1313,7 +1928,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="42"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -1352,7 +1967,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
+      <c r="A7" s="42"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -1391,7 +2006,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
+      <c r="A8" s="42"/>
       <c r="B8">
         <v>20</v>
       </c>
@@ -1430,17 +2045,17 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="42"/>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="47">
         <v>0.999966666666666</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="8">
         <v>0.999966666666666</v>
       </c>
@@ -1477,15 +2092,15 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
+      <c r="A10" s="42"/>
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="11"/>
@@ -1510,15 +2125,15 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+      <c r="A11" s="42"/>
       <c r="B11">
         <v>200</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="11"/>
@@ -1543,15 +2158,15 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="42"/>
       <c r="B12">
         <v>1000</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
@@ -1608,20 +2223,20 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="36" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
       <c r="K16" s="27"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -1633,8 +2248,8 @@
       <c r="S16" s="28"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="24" t="s">
         <v>13</v>
       </c>
@@ -1666,7 +2281,7 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="29">
@@ -1691,7 +2306,7 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="29">
         <v>100</v>
       </c>
@@ -1724,7 +2339,7 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="30">
         <v>200</v>
       </c>
@@ -1751,7 +2366,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="30">
         <v>500</v>
       </c>
@@ -1774,7 +2389,7 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="31">
         <v>1000</v>
       </c>
@@ -1793,7 +2408,7 @@
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="31">
         <v>2000</v>
       </c>
@@ -1812,7 +2427,7 @@
       <c r="K23" s="33"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="34"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1825,7 +2440,7 @@
       <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="31"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1978,7 +2593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>

</xml_diff>

<commit_message>
Combine downscaled luv and hog (best results)
</commit_message>
<xml_diff>
--- a/resultats/random_forest_gridsearch.xlsx
+++ b/resultats/random_forest_gridsearch.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Maximum features to consider</t>
   </si>
@@ -148,6 +148,12 @@
   <si>
     <t>Min samples split</t>
   </si>
+  <si>
+    <t>Min samples split = 2</t>
+  </si>
+  <si>
+    <t>Num est = 500</t>
+  </si>
 </sst>
 </file>
 
@@ -157,7 +163,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,6 +186,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -195,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -338,12 +360,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -395,11 +432,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,21 +483,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -460,19 +501,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -761,25 +802,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C2" s="38">
@@ -827,7 +868,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="47" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="38">
@@ -877,7 +918,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="38">
         <v>100</v>
       </c>
@@ -925,7 +966,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="38">
         <v>200</v>
       </c>
@@ -973,7 +1014,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="38">
         <v>500</v>
       </c>
@@ -1021,7 +1062,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="38">
         <v>1000</v>
       </c>
@@ -1069,7 +1110,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="38">
         <v>2000</v>
       </c>
@@ -1141,92 +1182,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="9" width="5.6640625" customWidth="1"/>
+    <col min="3" max="9" width="7.6640625" customWidth="1"/>
     <col min="10" max="10" width="3.1640625" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" customWidth="1"/>
-    <col min="12" max="15" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" customWidth="1"/>
+    <col min="13" max="17" width="8.1640625" customWidth="1"/>
+    <col min="18" max="18" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C1" s="39" t="s">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="56"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C2" s="51">
+      <c r="C2" s="39">
         <v>4</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="39">
         <v>6</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="39">
         <v>8</v>
       </c>
-      <c r="F2" s="51">
+      <c r="F2" s="39">
         <v>10</v>
       </c>
-      <c r="G2" s="51">
+      <c r="G2" s="39">
         <v>12</v>
       </c>
-      <c r="H2" s="51">
+      <c r="H2" s="39">
         <v>32</v>
       </c>
-      <c r="I2" s="51">
+      <c r="I2" s="39">
         <v>48</v>
       </c>
-      <c r="J2" s="57"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="51">
+      <c r="L2" s="39">
         <v>4</v>
       </c>
-      <c r="M2" s="51">
+      <c r="M2" s="39">
         <v>6</v>
       </c>
-      <c r="N2" s="51">
+      <c r="N2" s="39">
         <v>8</v>
       </c>
-      <c r="O2" s="51">
+      <c r="O2" s="39">
         <v>10</v>
       </c>
-      <c r="P2" s="51">
+      <c r="P2" s="39">
         <v>12</v>
       </c>
-      <c r="Q2" s="51">
+      <c r="Q2" s="39">
         <v>32</v>
       </c>
-      <c r="R2" s="51">
+      <c r="R2" s="39">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="47" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="38">
@@ -1280,7 +1325,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="38">
         <v>100</v>
       </c>
@@ -1332,7 +1377,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="38">
         <v>300</v>
       </c>
@@ -1384,8 +1429,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="52">
+      <c r="A6" s="47"/>
+      <c r="B6" s="40">
         <v>500</v>
       </c>
       <c r="C6" s="37">
@@ -1410,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="37"/>
-      <c r="K6" s="52">
+      <c r="K6" s="40">
         <v>500</v>
       </c>
       <c r="L6">
@@ -1430,8 +1475,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="52">
+      <c r="A7" s="47"/>
+      <c r="B7" s="40">
         <v>1000</v>
       </c>
       <c r="C7" s="37">
@@ -1456,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="37"/>
-      <c r="K7" s="52">
+      <c r="K7" s="40">
         <v>1000</v>
       </c>
       <c r="L7">
@@ -1476,7 +1521,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="38"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
@@ -1495,18 +1540,21 @@
       <c r="R8" s="36"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C10" s="54" t="s">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="L10" s="54" t="s">
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="L10" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C11" s="38">
@@ -1535,157 +1583,438 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="48" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="38">
         <v>2</v>
       </c>
-      <c r="C12" s="53">
-        <v>1</v>
-      </c>
-      <c r="D12" s="53">
-        <v>1</v>
-      </c>
-      <c r="E12" s="53">
-        <v>1</v>
-      </c>
-      <c r="F12" s="53">
-        <v>1</v>
-      </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="41">
+        <v>1</v>
+      </c>
+      <c r="E12" s="41">
+        <v>1</v>
+      </c>
+      <c r="F12" s="41">
+        <v>1</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
       <c r="K12" s="38">
         <v>2</v>
       </c>
-      <c r="L12" s="53">
+      <c r="L12" s="41">
         <v>0.535299999999999</v>
       </c>
-      <c r="M12" s="53">
+      <c r="M12" s="41">
         <v>0.53469999999999895</v>
       </c>
-      <c r="N12" s="53">
+      <c r="N12" s="41">
         <v>0.53759999999999897</v>
       </c>
-      <c r="O12" s="53">
+      <c r="O12" s="41">
         <v>0.53600000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="55"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="38">
         <v>4</v>
       </c>
-      <c r="C13" s="53">
-        <v>1</v>
-      </c>
-      <c r="D13" s="53">
-        <v>1</v>
-      </c>
-      <c r="E13" s="53">
-        <v>1</v>
-      </c>
-      <c r="F13" s="53">
-        <v>1</v>
-      </c>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="C13" s="41">
+        <v>1</v>
+      </c>
+      <c r="D13" s="41">
+        <v>1</v>
+      </c>
+      <c r="E13" s="41">
+        <v>1</v>
+      </c>
+      <c r="F13" s="41">
+        <v>1</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
       <c r="K13" s="38">
         <v>4</v>
       </c>
-      <c r="L13" s="53">
+      <c r="L13" s="41">
         <v>0.52880000000000005</v>
       </c>
-      <c r="M13" s="53">
+      <c r="M13" s="41">
         <v>0.53469999999999895</v>
       </c>
-      <c r="N13" s="53">
+      <c r="N13" s="41">
         <v>0.53649999999999898</v>
       </c>
-      <c r="O13" s="53">
+      <c r="O13" s="41">
         <v>0.53810000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="55"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="38">
         <v>8</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="41">
         <v>0.99882000000000004</v>
       </c>
-      <c r="D14" s="53">
+      <c r="D14" s="41">
         <v>0.99895999999999896</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="41">
         <v>0.99904000000000004</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="41">
         <v>0.99914000000000003</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
       <c r="K14" s="38">
         <v>8</v>
       </c>
-      <c r="L14" s="53">
+      <c r="L14" s="41">
         <v>0.52990000000000004</v>
       </c>
-      <c r="M14" s="53">
+      <c r="M14" s="41">
         <v>0.53010000000000002</v>
       </c>
-      <c r="N14" s="53">
+      <c r="N14" s="41">
         <v>0.53210000000000002</v>
       </c>
-      <c r="O14" s="53">
+      <c r="O14" s="41">
         <v>0.53210000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="55"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="38">
         <v>16</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="41">
         <v>0.96962000000000004</v>
       </c>
-      <c r="D15" s="53">
+      <c r="D15" s="41">
         <v>0.97206000000000004</v>
       </c>
-      <c r="E15" s="53">
+      <c r="E15" s="41">
         <v>0.97418000000000005</v>
       </c>
-      <c r="F15" s="53">
+      <c r="F15" s="41">
         <v>0.97543999999999897</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
       <c r="K15" s="38">
         <v>16</v>
       </c>
-      <c r="L15" s="53">
+      <c r="L15" s="41">
         <v>0.52239999999999898</v>
       </c>
-      <c r="M15" s="53">
+      <c r="M15" s="41">
         <v>0.522199999999999</v>
       </c>
-      <c r="N15" s="53">
+      <c r="N15" s="41">
         <v>0.52539999999999898</v>
       </c>
-      <c r="O15" s="53">
+      <c r="O15" s="41">
         <v>0.52449999999999897</v>
       </c>
     </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="M17" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C18" s="45"/>
+      <c r="D18" s="44">
+        <v>8</v>
+      </c>
+      <c r="E18" s="38">
+        <v>10</v>
+      </c>
+      <c r="F18" s="38">
+        <v>12</v>
+      </c>
+      <c r="G18" s="40">
+        <v>14</v>
+      </c>
+      <c r="H18" s="40">
+        <v>16</v>
+      </c>
+      <c r="L18" s="45"/>
+      <c r="M18" s="44">
+        <v>8</v>
+      </c>
+      <c r="N18" s="38">
+        <v>10</v>
+      </c>
+      <c r="O18" s="38">
+        <v>12</v>
+      </c>
+      <c r="P18" s="40">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="38">
+        <v>2</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41">
+        <v>1</v>
+      </c>
+      <c r="E19" s="41">
+        <v>1</v>
+      </c>
+      <c r="F19" s="41">
+        <v>1</v>
+      </c>
+      <c r="G19" s="41">
+        <v>1</v>
+      </c>
+      <c r="H19" s="41">
+        <v>1</v>
+      </c>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="38">
+        <v>2</v>
+      </c>
+      <c r="L19" s="41"/>
+      <c r="M19" s="36">
+        <v>0.55020000000000002</v>
+      </c>
+      <c r="N19" s="36">
+        <v>0.54830000000000001</v>
+      </c>
+      <c r="O19" s="36">
+        <v>0.5514</v>
+      </c>
+      <c r="P19" s="36">
+        <v>0.55059999999999898</v>
+      </c>
+      <c r="Q19" s="36">
+        <v>0.54610000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="48"/>
+      <c r="B20" s="38">
+        <v>4</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41">
+        <v>1</v>
+      </c>
+      <c r="E20" s="41">
+        <v>1</v>
+      </c>
+      <c r="F20" s="41">
+        <v>1</v>
+      </c>
+      <c r="G20" s="41">
+        <v>1</v>
+      </c>
+      <c r="H20" s="41">
+        <v>1</v>
+      </c>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="38">
+        <v>4</v>
+      </c>
+      <c r="L20" s="41"/>
+      <c r="M20" s="36">
+        <v>0.54869999999999897</v>
+      </c>
+      <c r="N20" s="36">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="O20" s="36">
+        <v>0.54479999999999895</v>
+      </c>
+      <c r="P20" s="36">
+        <v>0.54620000000000002</v>
+      </c>
+      <c r="Q20" s="36">
+        <v>0.54630000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="48"/>
+      <c r="B21" s="38">
+        <v>8</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41">
+        <v>0.99941999999999898</v>
+      </c>
+      <c r="E21" s="41">
+        <v>0.99956</v>
+      </c>
+      <c r="F21" s="41">
+        <v>0.99951999999999896</v>
+      </c>
+      <c r="G21" s="41">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="H21" s="41">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="38">
+        <v>8</v>
+      </c>
+      <c r="L21" s="41"/>
+      <c r="M21" s="36">
+        <v>0.54579999999999895</v>
+      </c>
+      <c r="N21" s="36">
+        <v>0.54249999999999898</v>
+      </c>
+      <c r="O21" s="36">
+        <v>0.54420000000000002</v>
+      </c>
+      <c r="P21" s="36">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="Q21" s="36">
+        <v>0.54369999999999896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="48"/>
+      <c r="B22" s="38">
+        <v>16</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41">
+        <v>0.98043999999999898</v>
+      </c>
+      <c r="E22" s="41">
+        <v>0.98182000000000003</v>
+      </c>
+      <c r="F22" s="41">
+        <v>0.98287999999999898</v>
+      </c>
+      <c r="G22" s="41">
+        <v>0.98292000000000002</v>
+      </c>
+      <c r="H22" s="41">
+        <v>0.98362000000000005</v>
+      </c>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="38">
+        <v>16</v>
+      </c>
+      <c r="L22" s="41"/>
+      <c r="M22" s="36">
+        <v>0.53480000000000005</v>
+      </c>
+      <c r="N22" s="36">
+        <v>0.53469999999999895</v>
+      </c>
+      <c r="O22" s="36">
+        <v>0.53569999999999895</v>
+      </c>
+      <c r="P22" s="36">
+        <v>0.53510000000000002</v>
+      </c>
+      <c r="Q22" s="36">
+        <v>0.53580000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M25" s="36">
+        <v>0.52980000000000005</v>
+      </c>
+      <c r="N25" s="36">
+        <v>0.52769999999999895</v>
+      </c>
+      <c r="O25" s="36">
+        <v>0.52910000000000001</v>
+      </c>
+      <c r="P25" s="36">
+        <v>0.53010000000000002</v>
+      </c>
+      <c r="Q25" s="36">
+        <v>0.53269999999999895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M26" s="36">
+        <v>0.53539999999999899</v>
+      </c>
+      <c r="N26" s="36">
+        <v>0.53080000000000005</v>
+      </c>
+      <c r="O26" s="36">
+        <v>0.53010000000000002</v>
+      </c>
+      <c r="P26" s="36">
+        <v>0.53280000000000005</v>
+      </c>
+      <c r="Q26" s="36">
+        <v>0.52969999999999895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M27" s="36">
+        <v>0.53039999999999898</v>
+      </c>
+      <c r="N27" s="36">
+        <v>0.52549999999999897</v>
+      </c>
+      <c r="O27" s="36">
+        <v>0.52929999999999899</v>
+      </c>
+      <c r="P27" s="36">
+        <v>0.53339999999999899</v>
+      </c>
+      <c r="Q27" s="36">
+        <v>0.532299999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="D17:H17"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="A3:A8"/>
@@ -1694,6 +2023,42 @@
     <mergeCell ref="A12:A15"/>
   </mergeCells>
   <conditionalFormatting sqref="L8:R8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:R7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:O15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:O22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1705,7 +2070,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:R7">
+  <conditionalFormatting sqref="M19:Q22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1717,7 +2082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L12:O15">
+  <conditionalFormatting sqref="M25:Q27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1730,6 +2095,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1753,48 +2119,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="45"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="54"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C3" s="23">
@@ -1848,7 +2214,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -1889,7 +2255,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="51"/>
       <c r="B5">
         <v>2</v>
       </c>
@@ -1928,7 +2294,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
+      <c r="A6" s="51"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -1967,7 +2333,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
+      <c r="A7" s="51"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -2006,7 +2372,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="51"/>
       <c r="B8">
         <v>20</v>
       </c>
@@ -2045,17 +2411,17 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="51"/>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="56">
         <v>0.999966666666666</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="8">
         <v>0.999966666666666</v>
       </c>
@@ -2092,15 +2458,15 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="51"/>
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="11"/>
@@ -2125,15 +2491,15 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="51"/>
       <c r="B11">
         <v>200</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="11"/>
@@ -2158,15 +2524,15 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="51"/>
       <c r="B12">
         <v>1000</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
@@ -2223,20 +2589,20 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="41" t="s">
+      <c r="B16" s="55"/>
+      <c r="C16" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
       <c r="K16" s="27"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -2248,8 +2614,8 @@
       <c r="S16" s="28"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="24" t="s">
         <v>13</v>
       </c>
@@ -2281,7 +2647,7 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="51" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="29">
@@ -2306,7 +2672,7 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="29">
         <v>100</v>
       </c>
@@ -2339,7 +2705,7 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="30">
         <v>200</v>
       </c>
@@ -2366,7 +2732,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="30">
         <v>500</v>
       </c>
@@ -2389,7 +2755,7 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="31">
         <v>1000</v>
       </c>
@@ -2408,7 +2774,7 @@
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="31">
         <v>2000</v>
       </c>
@@ -2427,7 +2793,7 @@
       <c r="K23" s="33"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="34"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2440,7 +2806,7 @@
       <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="31"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>

</xml_diff>

<commit_message>
Use a validation subset
</commit_message>
<xml_diff>
--- a/resultats/random_forest_gridsearch.xlsx
+++ b/resultats/random_forest_gridsearch.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Maximum features to consider</t>
   </si>
@@ -154,6 +154,12 @@
   <si>
     <t>Num est = 500</t>
   </si>
+  <si>
+    <t>Training accuracy</t>
+  </si>
+  <si>
+    <t>"Out of bag" score</t>
+  </si>
 </sst>
 </file>
 
@@ -163,7 +169,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,6 +208,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -217,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -373,6 +394,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -380,7 +425,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -481,6 +526,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -790,7 +850,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q8"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,24 +1242,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="3.1640625" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" customWidth="1"/>
-    <col min="13" max="17" width="8.1640625" customWidth="1"/>
-    <col min="18" max="18" width="7.83203125" customWidth="1"/>
+    <col min="3" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" customWidth="1"/>
+    <col min="13" max="18" width="8.1640625" customWidth="1"/>
+    <col min="19" max="19" width="7.83203125" customWidth="1"/>
+    <col min="20" max="25" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1213,18 +1274,19 @@
       <c r="H1" s="46"/>
       <c r="I1" s="46"/>
       <c r="J1" s="42"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="46" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="46"/>
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
       <c r="P1" s="46"/>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" s="46"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C2" s="39">
         <v>4</v>
       </c>
@@ -1247,30 +1309,31 @@
         <v>48</v>
       </c>
       <c r="J2" s="43"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="39">
+      <c r="K2" s="43"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="39">
         <v>4</v>
       </c>
-      <c r="M2" s="39">
+      <c r="N2" s="39">
         <v>6</v>
       </c>
-      <c r="N2" s="39">
+      <c r="O2" s="39">
         <v>8</v>
       </c>
-      <c r="O2" s="39">
+      <c r="P2" s="39">
         <v>10</v>
       </c>
-      <c r="P2" s="39">
+      <c r="Q2" s="39">
         <v>12</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="R2" s="39">
         <v>32</v>
       </c>
-      <c r="R2" s="39">
+      <c r="S2" s="39">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>20</v>
       </c>
@@ -1299,32 +1362,33 @@
         <v>0.99160000000000004</v>
       </c>
       <c r="J3" s="37"/>
-      <c r="K3" s="38">
+      <c r="K3" s="37"/>
+      <c r="L3" s="38">
         <v>10</v>
       </c>
-      <c r="L3" s="36">
+      <c r="M3" s="36">
         <v>0.40150000000000002</v>
       </c>
-      <c r="M3" s="36">
+      <c r="N3" s="36">
         <v>0.41049999999999898</v>
       </c>
-      <c r="N3" s="36">
+      <c r="O3" s="36">
         <v>0.40949999999999898</v>
       </c>
-      <c r="O3" s="36">
+      <c r="P3" s="36">
         <v>0.41170000000000001</v>
       </c>
-      <c r="P3" s="36">
+      <c r="Q3" s="36">
         <v>0.41589999999999899</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="R3" s="36">
         <v>0.42209999999999898</v>
       </c>
-      <c r="R3" s="36">
+      <c r="S3" s="36">
         <v>0.422899999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="47"/>
       <c r="B4" s="38">
         <v>100</v>
@@ -1351,32 +1415,33 @@
         <v>1</v>
       </c>
       <c r="J4" s="37"/>
-      <c r="K4" s="38">
+      <c r="K4" s="37"/>
+      <c r="L4" s="38">
         <v>100</v>
       </c>
-      <c r="L4" s="36">
+      <c r="M4" s="36">
         <v>0.51200000000000001</v>
       </c>
-      <c r="M4" s="36">
+      <c r="N4" s="36">
         <v>0.51470000000000005</v>
       </c>
-      <c r="N4" s="36">
+      <c r="O4" s="36">
         <v>0.51900000000000002</v>
       </c>
-      <c r="O4" s="36">
+      <c r="P4" s="36">
         <v>0.51839999999999897</v>
       </c>
-      <c r="P4" s="36">
+      <c r="Q4" s="36">
         <v>0.51580000000000004</v>
       </c>
-      <c r="Q4" s="36">
+      <c r="R4" s="36">
         <v>0.51659999999999895</v>
       </c>
-      <c r="R4" s="36">
+      <c r="S4" s="36">
         <v>0.50939999999999896</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="38">
         <v>300</v>
@@ -1403,32 +1468,33 @@
         <v>1</v>
       </c>
       <c r="J5" s="37"/>
-      <c r="K5" s="38">
+      <c r="K5" s="37"/>
+      <c r="L5" s="38">
         <v>300</v>
       </c>
-      <c r="L5" s="36">
+      <c r="M5" s="36">
         <v>0.53300000000000003</v>
       </c>
-      <c r="M5" s="36">
+      <c r="N5" s="36">
         <v>0.534299999999999</v>
       </c>
-      <c r="N5" s="36">
+      <c r="O5" s="36">
         <v>0.532299999999999</v>
       </c>
-      <c r="O5" s="36">
+      <c r="P5" s="36">
         <v>0.53469999999999895</v>
       </c>
-      <c r="P5" s="36">
+      <c r="Q5" s="36">
         <v>0.53149999999999897</v>
       </c>
-      <c r="Q5" s="36">
+      <c r="R5" s="36">
         <v>0.52549999999999897</v>
       </c>
-      <c r="R5" s="36">
+      <c r="S5" s="36">
         <v>0.52139999999999898</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="47"/>
       <c r="B6" s="40">
         <v>500</v>
@@ -1455,11 +1521,9 @@
         <v>1</v>
       </c>
       <c r="J6" s="37"/>
-      <c r="K6" s="40">
+      <c r="K6" s="37"/>
+      <c r="L6" s="40">
         <v>500</v>
-      </c>
-      <c r="L6">
-        <v>0.53500000000000003</v>
       </c>
       <c r="M6">
         <v>0.53500000000000003</v>
@@ -1468,13 +1532,16 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="O6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="P6">
         <v>0.53800000000000003</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="47"/>
       <c r="B7" s="40">
         <v>1000</v>
@@ -1501,26 +1568,27 @@
         <v>1</v>
       </c>
       <c r="J7" s="37"/>
-      <c r="K7" s="40">
+      <c r="K7" s="37"/>
+      <c r="L7" s="40">
         <v>1000</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.53500000000000003</v>
-      </c>
-      <c r="M7">
-        <v>0.53600000000000003</v>
       </c>
       <c r="N7">
         <v>0.53600000000000003</v>
       </c>
       <c r="O7">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="P7">
         <v>0.53700000000000003</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="47"/>
       <c r="B8" s="38"/>
       <c r="C8" s="37"/>
@@ -1531,15 +1599,16 @@
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
       <c r="J8" s="37"/>
-      <c r="L8" s="36"/>
+      <c r="K8" s="37"/>
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
       <c r="R8" s="36"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S8" s="36"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1549,14 +1618,14 @@
       <c r="D10" s="49"/>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
-      <c r="L10" s="49" t="s">
+      <c r="M10" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="49"/>
       <c r="N10" s="49"/>
       <c r="O10" s="49"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P10" s="49"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C11" s="38">
         <v>6</v>
       </c>
@@ -1569,20 +1638,20 @@
       <c r="F11" s="38">
         <v>12</v>
       </c>
-      <c r="L11" s="38">
+      <c r="M11" s="38">
         <v>6</v>
       </c>
-      <c r="M11" s="38">
+      <c r="N11" s="38">
         <v>8</v>
       </c>
-      <c r="N11" s="38">
+      <c r="O11" s="38">
         <v>10</v>
       </c>
-      <c r="O11" s="38">
+      <c r="P11" s="38">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
         <v>22</v>
       </c>
@@ -1605,23 +1674,24 @@
       <c r="H12" s="41"/>
       <c r="I12" s="41"/>
       <c r="J12" s="41"/>
-      <c r="K12" s="38">
+      <c r="K12" s="41"/>
+      <c r="L12" s="38">
         <v>2</v>
       </c>
-      <c r="L12" s="41">
+      <c r="M12" s="41">
         <v>0.535299999999999</v>
       </c>
-      <c r="M12" s="41">
+      <c r="N12" s="41">
         <v>0.53469999999999895</v>
       </c>
-      <c r="N12" s="41">
+      <c r="O12" s="41">
         <v>0.53759999999999897</v>
       </c>
-      <c r="O12" s="41">
+      <c r="P12" s="41">
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="38">
         <v>4</v>
@@ -1642,23 +1712,24 @@
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
-      <c r="K13" s="38">
+      <c r="K13" s="41"/>
+      <c r="L13" s="38">
         <v>4</v>
       </c>
-      <c r="L13" s="41">
+      <c r="M13" s="41">
         <v>0.52880000000000005</v>
       </c>
-      <c r="M13" s="41">
+      <c r="N13" s="41">
         <v>0.53469999999999895</v>
       </c>
-      <c r="N13" s="41">
+      <c r="O13" s="41">
         <v>0.53649999999999898</v>
       </c>
-      <c r="O13" s="41">
+      <c r="P13" s="41">
         <v>0.53810000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="38">
         <v>8</v>
@@ -1679,23 +1750,24 @@
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
       <c r="J14" s="41"/>
-      <c r="K14" s="38">
+      <c r="K14" s="41"/>
+      <c r="L14" s="38">
         <v>8</v>
       </c>
-      <c r="L14" s="41">
+      <c r="M14" s="41">
         <v>0.52990000000000004</v>
       </c>
-      <c r="M14" s="41">
+      <c r="N14" s="41">
         <v>0.53010000000000002</v>
-      </c>
-      <c r="N14" s="41">
-        <v>0.53210000000000002</v>
       </c>
       <c r="O14" s="41">
         <v>0.53210000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P14" s="41">
+        <v>0.53210000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="48"/>
       <c r="B15" s="38">
         <v>16</v>
@@ -1716,23 +1788,24 @@
       <c r="H15" s="41"/>
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
-      <c r="K15" s="38">
+      <c r="K15" s="41"/>
+      <c r="L15" s="38">
         <v>16</v>
       </c>
-      <c r="L15" s="41">
+      <c r="M15" s="41">
         <v>0.52239999999999898</v>
       </c>
-      <c r="M15" s="41">
+      <c r="N15" s="41">
         <v>0.522199999999999</v>
       </c>
-      <c r="N15" s="41">
+      <c r="O15" s="41">
         <v>0.52539999999999898</v>
       </c>
-      <c r="O15" s="41">
+      <c r="P15" s="41">
         <v>0.52449999999999897</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1743,15 +1816,15 @@
       <c r="F17" s="49"/>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
-      <c r="M17" s="49" t="s">
+      <c r="N17" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="N17" s="49"/>
       <c r="O17" s="49"/>
       <c r="P17" s="49"/>
       <c r="Q17" s="49"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" s="49"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C18" s="45"/>
       <c r="D18" s="44">
         <v>8</v>
@@ -1768,24 +1841,24 @@
       <c r="H18" s="40">
         <v>16</v>
       </c>
-      <c r="L18" s="45"/>
-      <c r="M18" s="44">
+      <c r="M18" s="45"/>
+      <c r="N18" s="44">
         <v>8</v>
       </c>
-      <c r="N18" s="38">
+      <c r="O18" s="38">
         <v>10</v>
       </c>
-      <c r="O18" s="38">
+      <c r="P18" s="38">
         <v>12</v>
       </c>
-      <c r="P18" s="40">
+      <c r="Q18" s="40">
         <v>14</v>
       </c>
-      <c r="Q18" s="40">
+      <c r="R18" s="40">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
         <v>22</v>
       </c>
@@ -1810,27 +1883,28 @@
       </c>
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
-      <c r="K19" s="38">
+      <c r="K19" s="41"/>
+      <c r="L19" s="38">
         <v>2</v>
       </c>
-      <c r="L19" s="41"/>
-      <c r="M19" s="36">
+      <c r="M19" s="41"/>
+      <c r="N19" s="36">
         <v>0.55020000000000002</v>
       </c>
-      <c r="N19" s="36">
+      <c r="O19" s="36">
         <v>0.54830000000000001</v>
       </c>
-      <c r="O19" s="36">
+      <c r="P19" s="36">
         <v>0.5514</v>
       </c>
-      <c r="P19" s="36">
+      <c r="Q19" s="36">
         <v>0.55059999999999898</v>
       </c>
-      <c r="Q19" s="36">
+      <c r="R19" s="36">
         <v>0.54610000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
       <c r="B20" s="38">
         <v>4</v>
@@ -1853,27 +1927,28 @@
       </c>
       <c r="I20" s="41"/>
       <c r="J20" s="41"/>
-      <c r="K20" s="38">
+      <c r="K20" s="41"/>
+      <c r="L20" s="38">
         <v>4</v>
       </c>
-      <c r="L20" s="41"/>
-      <c r="M20" s="36">
+      <c r="M20" s="41"/>
+      <c r="N20" s="36">
         <v>0.54869999999999897</v>
       </c>
-      <c r="N20" s="36">
+      <c r="O20" s="36">
         <v>0.54900000000000004</v>
       </c>
-      <c r="O20" s="36">
+      <c r="P20" s="36">
         <v>0.54479999999999895</v>
       </c>
-      <c r="P20" s="36">
+      <c r="Q20" s="36">
         <v>0.54620000000000002</v>
       </c>
-      <c r="Q20" s="36">
+      <c r="R20" s="36">
         <v>0.54630000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
       <c r="B21" s="38">
         <v>8</v>
@@ -1896,27 +1971,28 @@
       </c>
       <c r="I21" s="41"/>
       <c r="J21" s="41"/>
-      <c r="K21" s="38">
+      <c r="K21" s="41"/>
+      <c r="L21" s="38">
         <v>8</v>
       </c>
-      <c r="L21" s="41"/>
-      <c r="M21" s="36">
+      <c r="M21" s="41"/>
+      <c r="N21" s="36">
         <v>0.54579999999999895</v>
       </c>
-      <c r="N21" s="36">
+      <c r="O21" s="36">
         <v>0.54249999999999898</v>
       </c>
-      <c r="O21" s="36">
+      <c r="P21" s="36">
         <v>0.54420000000000002</v>
       </c>
-      <c r="P21" s="36">
+      <c r="Q21" s="36">
         <v>0.54300000000000004</v>
       </c>
-      <c r="Q21" s="36">
+      <c r="R21" s="36">
         <v>0.54369999999999896</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="48"/>
       <c r="B22" s="38">
         <v>16</v>
@@ -1939,91 +2015,604 @@
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="41"/>
-      <c r="K22" s="38">
+      <c r="K22" s="41"/>
+      <c r="L22" s="38">
         <v>16</v>
       </c>
-      <c r="L22" s="41"/>
-      <c r="M22" s="36">
+      <c r="M22" s="41"/>
+      <c r="N22" s="36">
         <v>0.53480000000000005</v>
       </c>
-      <c r="N22" s="36">
+      <c r="O22" s="36">
         <v>0.53469999999999895</v>
       </c>
-      <c r="O22" s="36">
+      <c r="P22" s="36">
         <v>0.53569999999999895</v>
       </c>
-      <c r="P22" s="36">
+      <c r="Q22" s="36">
         <v>0.53510000000000002</v>
       </c>
-      <c r="Q22" s="36">
+      <c r="R22" s="36">
         <v>0.53580000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="M25" s="36">
-        <v>0.52980000000000005</v>
-      </c>
-      <c r="N25" s="36">
-        <v>0.52769999999999895</v>
-      </c>
-      <c r="O25" s="36">
-        <v>0.52910000000000001</v>
-      </c>
-      <c r="P25" s="36">
-        <v>0.53010000000000002</v>
-      </c>
-      <c r="Q25" s="36">
-        <v>0.53269999999999895</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="M26" s="36">
-        <v>0.53539999999999899</v>
-      </c>
-      <c r="N26" s="36">
-        <v>0.53080000000000005</v>
-      </c>
-      <c r="O26" s="36">
-        <v>0.53010000000000002</v>
-      </c>
-      <c r="P26" s="36">
-        <v>0.53280000000000005</v>
-      </c>
-      <c r="Q26" s="36">
-        <v>0.52969999999999895</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="52" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:25" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="S24" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="T24" s="64"/>
+      <c r="U24" s="64"/>
+      <c r="V24" s="64"/>
+      <c r="W24" s="64"/>
+      <c r="X24" s="64"/>
+      <c r="Y24" s="64"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="62"/>
+      <c r="M25" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="36"/>
+      <c r="U25" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="V25" s="46"/>
+      <c r="W25" s="46"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="46"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="E26" s="38">
+        <v>4</v>
+      </c>
+      <c r="F26" s="38">
+        <v>8</v>
+      </c>
+      <c r="G26" s="38">
+        <v>16</v>
+      </c>
+      <c r="H26" s="38">
+        <v>32</v>
+      </c>
+      <c r="I26" s="38">
+        <v>64</v>
+      </c>
+      <c r="M26" s="38">
+        <v>4</v>
+      </c>
+      <c r="N26" s="38">
+        <v>8</v>
+      </c>
+      <c r="O26" s="38">
+        <v>16</v>
+      </c>
+      <c r="P26" s="38">
+        <v>32</v>
+      </c>
+      <c r="Q26" s="38">
+        <v>64</v>
+      </c>
+      <c r="R26" s="36"/>
+      <c r="U26" s="38">
+        <v>4</v>
+      </c>
+      <c r="V26" s="38">
+        <v>8</v>
+      </c>
+      <c r="W26" s="38">
+        <v>16</v>
+      </c>
+      <c r="X26" s="38">
+        <v>32</v>
+      </c>
+      <c r="Y26" s="38">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C27" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="38">
+        <v>2</v>
+      </c>
+      <c r="E27" s="36">
+        <v>1</v>
+      </c>
+      <c r="F27" s="36">
+        <v>1</v>
+      </c>
+      <c r="G27" s="36">
+        <v>1</v>
+      </c>
+      <c r="H27" s="36">
+        <v>1</v>
+      </c>
+      <c r="I27" s="36">
+        <v>1</v>
+      </c>
+      <c r="K27" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="38">
+        <v>2</v>
+      </c>
       <c r="M27" s="36">
-        <v>0.53039999999999898</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="N27" s="36">
-        <v>0.52549999999999897</v>
+        <v>0.5635</v>
       </c>
       <c r="O27" s="36">
-        <v>0.52929999999999899</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="P27" s="36">
-        <v>0.53339999999999899</v>
+        <v>0.55889999999999895</v>
       </c>
       <c r="Q27" s="36">
-        <v>0.532299999999999</v>
+        <v>0.56020000000000003</v>
+      </c>
+      <c r="R27" s="36"/>
+      <c r="S27" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="T27" s="38">
+        <v>2</v>
+      </c>
+      <c r="U27">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="V27">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="W27">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="X27">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="Y27">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C28" s="47"/>
+      <c r="D28" s="38">
+        <v>4</v>
+      </c>
+      <c r="E28" s="36">
+        <v>1</v>
+      </c>
+      <c r="F28" s="36">
+        <v>1</v>
+      </c>
+      <c r="G28" s="36">
+        <v>1</v>
+      </c>
+      <c r="H28" s="36">
+        <v>1</v>
+      </c>
+      <c r="I28" s="36">
+        <v>1</v>
+      </c>
+      <c r="K28" s="47"/>
+      <c r="L28" s="38">
+        <v>4</v>
+      </c>
+      <c r="M28" s="36">
+        <v>0.55679999999999896</v>
+      </c>
+      <c r="N28" s="36">
+        <v>0.56169999999999898</v>
+      </c>
+      <c r="O28" s="36">
+        <v>0.56389999999999896</v>
+      </c>
+      <c r="P28" s="36">
+        <v>0.55789999999999895</v>
+      </c>
+      <c r="Q28" s="36">
+        <v>0.55220000000000002</v>
+      </c>
+      <c r="S28" s="47"/>
+      <c r="T28" s="38">
+        <v>4</v>
+      </c>
+      <c r="U28">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="V28">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="W28">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="X28">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="Y28">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C29" s="47"/>
+      <c r="D29" s="38">
+        <v>6</v>
+      </c>
+      <c r="E29" s="36">
+        <v>1</v>
+      </c>
+      <c r="F29" s="36">
+        <v>0.99997499999999895</v>
+      </c>
+      <c r="G29" s="36">
+        <v>0.99997499999999895</v>
+      </c>
+      <c r="H29" s="36">
+        <v>0.99997499999999895</v>
+      </c>
+      <c r="I29" s="36">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="K29" s="47"/>
+      <c r="L29" s="38">
+        <v>6</v>
+      </c>
+      <c r="M29" s="36">
+        <v>0.56410000000000005</v>
+      </c>
+      <c r="N29" s="36">
+        <v>0.55979999999999897</v>
+      </c>
+      <c r="O29" s="36">
+        <v>0.55759999999999899</v>
+      </c>
+      <c r="P29" s="36">
+        <v>0.556499999999999</v>
+      </c>
+      <c r="Q29" s="36">
+        <v>0.55489999999999895</v>
+      </c>
+      <c r="S29" s="47"/>
+      <c r="T29" s="38">
+        <v>6</v>
+      </c>
+      <c r="U29">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="V29">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="W29">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="X29">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="Y29">
+        <v>0.55800000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C30" s="47"/>
+      <c r="D30" s="38">
+        <v>8</v>
+      </c>
+      <c r="E30" s="36">
+        <v>0.99972499999999898</v>
+      </c>
+      <c r="F30" s="36">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G30" s="36">
+        <v>0.99987499999999896</v>
+      </c>
+      <c r="H30" s="36">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="I30" s="36">
+        <v>0.99975000000000003</v>
+      </c>
+      <c r="K30" s="47"/>
+      <c r="L30" s="38">
+        <v>8</v>
+      </c>
+      <c r="M30" s="36">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N30" s="36">
+        <v>0.55759999999999899</v>
+      </c>
+      <c r="O30" s="36">
+        <v>0.55720000000000003</v>
+      </c>
+      <c r="P30" s="36">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="Q30" s="36">
+        <v>0.55279999999999896</v>
+      </c>
+      <c r="S30" s="47"/>
+      <c r="T30" s="38">
+        <v>8</v>
+      </c>
+      <c r="U30">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="V30">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="W30">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="X30">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="Y30">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C31" s="47"/>
+      <c r="D31" s="38">
+        <v>10</v>
+      </c>
+      <c r="E31" s="36">
+        <v>0.99885000000000002</v>
+      </c>
+      <c r="F31" s="36">
+        <v>0.99909999999999899</v>
+      </c>
+      <c r="G31" s="36">
+        <v>0.99914999999999898</v>
+      </c>
+      <c r="H31" s="36">
+        <v>0.99939999999999896</v>
+      </c>
+      <c r="I31" s="36">
+        <v>0.99929999999999897</v>
+      </c>
+      <c r="K31" s="47"/>
+      <c r="L31" s="38">
+        <v>10</v>
+      </c>
+      <c r="M31" s="36">
+        <v>0.55589999999999895</v>
+      </c>
+      <c r="N31" s="36">
+        <v>0.5554</v>
+      </c>
+      <c r="O31" s="36">
+        <v>0.55589999999999895</v>
+      </c>
+      <c r="P31" s="36">
+        <v>0.55589999999999895</v>
+      </c>
+      <c r="Q31" s="36">
+        <v>0.55059999999999898</v>
+      </c>
+      <c r="S31" s="47"/>
+      <c r="T31" s="38">
+        <v>10</v>
+      </c>
+      <c r="U31">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="V31">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="W31">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="X31">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="Y31">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>0.55800000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <v>0.55800000000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <v>0.55500000000000005</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
+    <mergeCell ref="S24:Y24"/>
+    <mergeCell ref="U25:Y25"/>
+    <mergeCell ref="S27:S31"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="K24:Q24"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="N17:R17"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="M1:S1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="C10:F10"/>
-    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="M10:P10"/>
     <mergeCell ref="A12:A15"/>
   </mergeCells>
-  <conditionalFormatting sqref="L8:R8">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="M8:S8">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2034,7 +2623,67 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:R7">
+  <conditionalFormatting sqref="M5:S7">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12:P15">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M19:P22">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:R22">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25:R27">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:Q34">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2046,7 +2695,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L12:O15">
+  <conditionalFormatting sqref="M27:Q31">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2058,7 +2707,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19:O22">
+  <conditionalFormatting sqref="E27:I31">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2066,24 +2715,12 @@
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19:Q22">
+  <conditionalFormatting sqref="U27:Y31">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M25:Q27">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Get confusion matrix for best result on cifar10 with random forests
</commit_message>
<xml_diff>
--- a/resultats/random_forest_gridsearch.xlsx
+++ b/resultats/random_forest_gridsearch.xlsx
@@ -9,32 +9,34 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="MNIST-SIFT" sheetId="1" r:id="rId1"/>
+    <sheet name="BEST" sheetId="8" r:id="rId1"/>
     <sheet name="CIFAR10-GRAY" sheetId="7" r:id="rId2"/>
     <sheet name="CIFAR10-RGB" sheetId="5" r:id="rId3"/>
     <sheet name="CIFAR10-DSHOG" sheetId="4" r:id="rId4"/>
     <sheet name="CIFAR10-HOGBOW" sheetId="6" r:id="rId5"/>
     <sheet name="CIFAR10-HOG" sheetId="3" r:id="rId6"/>
+    <sheet name="MNIST-SIFT" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="confusion_rf" localSheetId="0">BEST!$C$6:$L$15</definedName>
     <definedName name="gridsearch_accuracy_oob" localSheetId="4">'CIFAR10-HOGBOW'!$T$10:$U$11</definedName>
     <definedName name="gridsearch_accuracy_oob_1" localSheetId="1">'CIFAR10-GRAY'!$AD$4:$AE$7</definedName>
     <definedName name="gridsearch_accuracy_oob_1" localSheetId="4">'CIFAR10-HOGBOW'!$Q$5:$S$9</definedName>
     <definedName name="gridsearch_accuracy_oob_2" localSheetId="4">'CIFAR10-HOGBOW'!$Q$10:$S$11</definedName>
     <definedName name="gridsearch_accuracy_oob_3" localSheetId="4">'CIFAR10-HOGBOW'!$T$5:$U$9</definedName>
     <definedName name="gridsearch_accuracy_test" localSheetId="4">'CIFAR10-HOGBOW'!$J$5:$L$9</definedName>
-    <definedName name="gridsearch_accuracy_test" localSheetId="0">'MNIST-SIFT'!$P$4:$S$9</definedName>
+    <definedName name="gridsearch_accuracy_test" localSheetId="6">'MNIST-SIFT'!$P$4:$S$9</definedName>
     <definedName name="gridsearch_accuracy_test_1" localSheetId="1">'CIFAR10-GRAY'!$T$4:$U$7</definedName>
     <definedName name="gridsearch_accuracy_test_1" localSheetId="4">'CIFAR10-HOGBOW'!$M$10:$N$11</definedName>
-    <definedName name="gridsearch_accuracy_test_1" localSheetId="0">'MNIST-SIFT'!$L$9:$P$12</definedName>
+    <definedName name="gridsearch_accuracy_test_1" localSheetId="6">'MNIST-SIFT'!$L$9:$P$12</definedName>
     <definedName name="gridsearch_accuracy_test_2" localSheetId="4">'CIFAR10-HOGBOW'!$J$10:$L$11</definedName>
-    <definedName name="gridsearch_accuracy_test_2" localSheetId="0">'MNIST-SIFT'!$C$21:$D$23</definedName>
+    <definedName name="gridsearch_accuracy_test_2" localSheetId="6">'MNIST-SIFT'!$C$21:$D$23</definedName>
     <definedName name="gridsearch_accuracy_test_3" localSheetId="4">'CIFAR10-HOGBOW'!$M$5:$N$9</definedName>
     <definedName name="gridsearch_accuracy_train" localSheetId="4">'CIFAR10-HOGBOW'!$C$5:$E$9</definedName>
-    <definedName name="gridsearch_accuracy_train" localSheetId="0">'MNIST-SIFT'!$G$4:$J$9</definedName>
+    <definedName name="gridsearch_accuracy_train" localSheetId="6">'MNIST-SIFT'!$G$4:$J$9</definedName>
     <definedName name="gridsearch_accuracy_train_1" localSheetId="1">'CIFAR10-GRAY'!$J$4:$K$7</definedName>
     <definedName name="gridsearch_accuracy_train_1" localSheetId="4">'CIFAR10-HOGBOW'!$F$10:$G$11</definedName>
     <definedName name="gridsearch_accuracy_train_2" localSheetId="4">'CIFAR10-HOGBOW'!$C$10:$E$11</definedName>
@@ -54,7 +56,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="gridsearch_accuracy_oob" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="confusion_rf" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/confusion_rf.csv" thousands=" " space="1" consecutive="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="gridsearch_accuracy_oob" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -62,7 +80,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="gridsearch_accuracy_oob1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="gridsearch_accuracy_oob1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="5">
         <textField/>
@@ -73,7 +91,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="gridsearch_accuracy_oob2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="gridsearch_accuracy_oob2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -82,7 +100,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="gridsearch_accuracy_oob3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="gridsearch_accuracy_oob3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -90,7 +108,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="gridsearch_accuracy_oob4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="gridsearch_accuracy_oob4" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -98,7 +116,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="gridsearch_accuracy_test" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="gridsearch_accuracy_test" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" " comma="1" semicolon="1">
       <textFields count="2">
         <textField/>
@@ -106,7 +124,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="gridsearch_accuracy_test1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="gridsearch_accuracy_test1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" " semicolon="1">
       <textFields count="3">
         <textField/>
@@ -115,7 +133,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="gridsearch_accuracy_test2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="gridsearch_accuracy_test2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="5">
         <textField/>
@@ -126,7 +144,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="gridsearch_accuracy_test3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" name="gridsearch_accuracy_test3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -134,7 +152,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="gridsearch_accuracy_test4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="gridsearch_accuracy_test4" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -143,7 +161,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="gridsearch_accuracy_test5" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="12" name="gridsearch_accuracy_test5" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -151,7 +169,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="gridsearch_accuracy_test6" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="13" name="gridsearch_accuracy_test6" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -159,7 +177,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="gridsearch_accuracy_train" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="14" name="gridsearch_accuracy_train" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" " comma="1" semicolon="1">
       <textFields count="3">
         <textField/>
@@ -168,7 +186,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="gridsearch_accuracy_train1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="15" name="gridsearch_accuracy_train1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -176,7 +194,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="gridsearch_accuracy_train2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="16" name="gridsearch_accuracy_train2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="5">
         <textField/>
@@ -187,7 +205,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="gridsearch_accuracy_train3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="17" name="gridsearch_accuracy_train3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -195,7 +213,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="gridsearch_accuracy_train4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="18" name="gridsearch_accuracy_train4" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -204,7 +222,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" name="gridsearch_accuracy_train5" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="19" name="gridsearch_accuracy_train5" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -216,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Maximum features to consider</t>
   </si>
@@ -328,6 +346,63 @@
   <si>
     <t>N. est</t>
   </si>
+  <si>
+    <t xml:space="preserve">airplane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">automobile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bird </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">deer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dog </t>
+  </si>
+  <si>
+    <t xml:space="preserve">frog </t>
+  </si>
+  <si>
+    <t xml:space="preserve">horse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ship </t>
+  </si>
+  <si>
+    <t>truck</t>
+  </si>
+  <si>
+    <t>Prédiction</t>
+  </si>
+  <si>
+    <t>Réel</t>
+  </si>
+  <si>
+    <t>Matrice de confusion</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Downsampled (facteur 8) en couleurs Luv, concaténé avec HOG (6 orientations, 4 blocs par dimension)</t>
+  </si>
+  <si>
+    <t>(Test accuracy)</t>
+  </si>
+  <si>
+    <t>Les couleurs sont affectées linéairement, avec la plus petite valeur en vert et la plus grande en rouge (la diagonale est exclue)</t>
+  </si>
+  <si>
+    <t>100% training accuracy</t>
+  </si>
+  <si>
+    <t>Meilleur résultat sur CIFAR10 avec Random Forest :</t>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +414,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -410,6 +485,21 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -664,7 +754,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -730,6 +820,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -805,7 +898,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -814,11 +906,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
@@ -841,79 +945,83 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion_rf" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_3" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_3" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_3" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_3" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_3" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_2" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_3" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1179,857 +1287,476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="9" width="8.1640625" customWidth="1"/>
-    <col min="10" max="13" width="7.83203125" customWidth="1"/>
-    <col min="14" max="15" width="8.6640625" customWidth="1"/>
-    <col min="16" max="19" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C2" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="56"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C3" s="22">
-        <v>2</v>
-      </c>
-      <c r="D3" s="23">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="E1" s="81">
+        <v>0.57889999999999997</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="86"/>
+      <c r="C4" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="86"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="25">
+        <v>627</v>
+      </c>
+      <c r="D6" s="25">
+        <v>42</v>
+      </c>
+      <c r="E6" s="25">
+        <v>42</v>
+      </c>
+      <c r="F6" s="25">
+        <v>30</v>
+      </c>
+      <c r="G6" s="25">
+        <v>12</v>
+      </c>
+      <c r="H6" s="25">
+        <v>9</v>
+      </c>
+      <c r="I6" s="25">
+        <v>25</v>
+      </c>
+      <c r="J6" s="25">
+        <v>20</v>
+      </c>
+      <c r="K6" s="25">
+        <v>137</v>
+      </c>
+      <c r="L6" s="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="85"/>
+      <c r="B7" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="25">
+        <v>41</v>
+      </c>
+      <c r="D7" s="25">
+        <v>720</v>
+      </c>
+      <c r="E7" s="25">
+        <v>6</v>
+      </c>
+      <c r="F7" s="25">
+        <v>13</v>
+      </c>
+      <c r="G7" s="25">
+        <v>19</v>
+      </c>
+      <c r="H7" s="25">
         <v>4</v>
       </c>
-      <c r="E3" s="23">
+      <c r="I7" s="25">
+        <v>24</v>
+      </c>
+      <c r="J7" s="25">
+        <v>6</v>
+      </c>
+      <c r="K7" s="25">
+        <v>65</v>
+      </c>
+      <c r="L7" s="25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="85"/>
+      <c r="B8" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="25">
+        <v>98</v>
+      </c>
+      <c r="D8" s="25">
+        <v>30</v>
+      </c>
+      <c r="E8" s="25">
+        <v>352</v>
+      </c>
+      <c r="F8" s="25">
+        <v>87</v>
+      </c>
+      <c r="G8" s="25">
+        <v>100</v>
+      </c>
+      <c r="H8" s="25">
+        <v>91</v>
+      </c>
+      <c r="I8" s="25">
+        <v>118</v>
+      </c>
+      <c r="J8" s="25">
+        <v>62</v>
+      </c>
+      <c r="K8" s="25">
+        <v>41</v>
+      </c>
+      <c r="L8" s="25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="85"/>
+      <c r="B9" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="25">
+        <v>29</v>
+      </c>
+      <c r="D9" s="25">
+        <v>37</v>
+      </c>
+      <c r="E9" s="25">
+        <v>36</v>
+      </c>
+      <c r="F9" s="25">
+        <v>445</v>
+      </c>
+      <c r="G9" s="25">
+        <v>44</v>
+      </c>
+      <c r="H9" s="25">
+        <v>181</v>
+      </c>
+      <c r="I9" s="25">
+        <v>116</v>
+      </c>
+      <c r="J9" s="25">
+        <v>44</v>
+      </c>
+      <c r="K9" s="25">
+        <v>18</v>
+      </c>
+      <c r="L9" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="85"/>
+      <c r="B10" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="25">
+        <v>37</v>
+      </c>
+      <c r="D10" s="25">
+        <v>17</v>
+      </c>
+      <c r="E10" s="25">
+        <v>52</v>
+      </c>
+      <c r="F10" s="25">
+        <v>99</v>
+      </c>
+      <c r="G10" s="25">
+        <v>456</v>
+      </c>
+      <c r="H10" s="25">
+        <v>48</v>
+      </c>
+      <c r="I10" s="25">
+        <v>137</v>
+      </c>
+      <c r="J10" s="25">
+        <v>98</v>
+      </c>
+      <c r="K10" s="25">
+        <v>29</v>
+      </c>
+      <c r="L10" s="25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="85"/>
+      <c r="B11" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="25">
+        <v>12</v>
+      </c>
+      <c r="D11" s="25">
+        <v>23</v>
+      </c>
+      <c r="E11" s="25">
+        <v>40</v>
+      </c>
+      <c r="F11" s="25">
+        <v>178</v>
+      </c>
+      <c r="G11" s="25">
+        <v>58</v>
+      </c>
+      <c r="H11" s="25">
+        <v>458</v>
+      </c>
+      <c r="I11" s="25">
+        <v>109</v>
+      </c>
+      <c r="J11" s="25">
+        <v>72</v>
+      </c>
+      <c r="K11" s="25">
+        <v>27</v>
+      </c>
+      <c r="L11" s="25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="85"/>
+      <c r="B12" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="25">
+        <v>6</v>
+      </c>
+      <c r="D12" s="25">
+        <v>17</v>
+      </c>
+      <c r="E12" s="25">
+        <v>45</v>
+      </c>
+      <c r="F12" s="25">
+        <v>67</v>
+      </c>
+      <c r="G12" s="25">
+        <v>62</v>
+      </c>
+      <c r="H12" s="25">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25">
+        <v>720</v>
+      </c>
+      <c r="J12" s="25">
+        <v>16</v>
+      </c>
+      <c r="K12" s="25">
+        <v>11</v>
+      </c>
+      <c r="L12" s="25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="85"/>
+      <c r="B13" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="25">
+        <v>19</v>
+      </c>
+      <c r="D13" s="25">
+        <v>17</v>
+      </c>
+      <c r="E13" s="25">
+        <v>22</v>
+      </c>
+      <c r="F13" s="25">
+        <v>76</v>
+      </c>
+      <c r="G13" s="25">
+        <v>64</v>
+      </c>
+      <c r="H13" s="25">
+        <v>87</v>
+      </c>
+      <c r="I13" s="25">
+        <v>33</v>
+      </c>
+      <c r="J13" s="25">
+        <v>619</v>
+      </c>
+      <c r="K13" s="25">
+        <v>17</v>
+      </c>
+      <c r="L13" s="25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="85"/>
+      <c r="B14" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="25">
+        <v>68</v>
+      </c>
+      <c r="D14" s="25">
+        <v>93</v>
+      </c>
+      <c r="E14" s="25">
+        <v>9</v>
+      </c>
+      <c r="F14" s="25">
+        <v>12</v>
+      </c>
+      <c r="G14" s="25">
+        <v>7</v>
+      </c>
+      <c r="H14" s="25">
+        <v>7</v>
+      </c>
+      <c r="I14" s="25">
         <v>8</v>
       </c>
-      <c r="F3" s="23">
-        <v>16</v>
-      </c>
-      <c r="G3" s="23">
-        <v>32</v>
-      </c>
-      <c r="H3" s="23">
-        <v>64</v>
-      </c>
-      <c r="I3" s="23">
-        <v>128</v>
-      </c>
-      <c r="J3" s="24">
-        <v>256</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="22">
-        <v>2</v>
-      </c>
-      <c r="M3" s="23">
-        <v>4</v>
-      </c>
-      <c r="N3" s="23">
-        <v>8</v>
-      </c>
-      <c r="O3" s="23">
-        <v>16</v>
-      </c>
-      <c r="P3" s="23">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="23">
-        <v>64</v>
-      </c>
-      <c r="R3" s="23">
-        <v>128</v>
-      </c>
-      <c r="S3" s="24">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="7">
-        <v>0.85303333333333298</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.86468333333333303</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0.86431666666666596</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.86809999999999898</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="7">
-        <v>0.60880000000000001</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>0.63260000000000005</v>
-      </c>
-      <c r="R4" s="7">
-        <v>0.633099999999999</v>
-      </c>
-      <c r="S4" s="8">
-        <v>0.64539999999999897</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="53"/>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="7">
-        <v>0.85394999999999899</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.86486666666666601</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0.86548333333333305</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.86916666666666598</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="7">
-        <v>0.60140000000000005</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>0.62539999999999896</v>
-      </c>
-      <c r="R5" s="7">
-        <v>0.63380000000000003</v>
-      </c>
-      <c r="S5" s="8">
-        <v>0.637099999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="7">
-        <v>0.97594999999999898</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.97423333333333295</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0.97135000000000005</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0.96968333333333301</v>
-      </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="7">
-        <v>0.72030000000000005</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>0.72250000000000003</v>
-      </c>
-      <c r="R6" s="7">
-        <v>0.72250000000000003</v>
-      </c>
-      <c r="S6" s="8">
-        <v>0.71379999999999899</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
-      <c r="B7">
+      <c r="J14" s="25">
+        <v>13</v>
+      </c>
+      <c r="K14" s="25">
+        <v>703</v>
+      </c>
+      <c r="L14" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="85"/>
+      <c r="B15" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="25">
+        <v>33</v>
+      </c>
+      <c r="D15" s="25">
+        <v>114</v>
+      </c>
+      <c r="E15" s="25">
+        <v>6</v>
+      </c>
+      <c r="F15" s="25">
+        <v>21</v>
+      </c>
+      <c r="G15" s="25">
+        <v>13</v>
+      </c>
+      <c r="H15" s="25">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="7">
-        <v>0.99546666666666594</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.99460000000000004</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0.99273333333333302</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0.99099999999999899</v>
-      </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="7">
-        <v>0.7671</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>0.76559999999999895</v>
-      </c>
-      <c r="R7" s="7">
-        <v>0.75509999999999899</v>
-      </c>
-      <c r="S7" s="8">
-        <v>0.74829999999999897</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
-      <c r="B8">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="7">
-        <v>0.99944999999999895</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0.99928333333333297</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0.99861666666666604</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0.99804999999999899</v>
-      </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="7">
-        <v>0.79859999999999898</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>0.78459999999999896</v>
-      </c>
-      <c r="R8" s="7">
-        <v>0.77629999999999899</v>
-      </c>
-      <c r="S8" s="8">
-        <v>0.76370000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9">
-        <v>50</v>
-      </c>
-      <c r="C9" s="58">
-        <v>0.999966666666666</v>
-      </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="7">
-        <v>0.999966666666666</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0.99978333333333302</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="13">
-        <v>0.83620000000000005</v>
-      </c>
-      <c r="M9" s="14">
-        <v>0.83309999999999895</v>
-      </c>
-      <c r="N9" s="14">
-        <v>0.83640000000000003</v>
-      </c>
-      <c r="O9" s="14">
-        <v>0.82730000000000004</v>
-      </c>
-      <c r="P9" s="14">
-        <v>0.81630000000000003</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>0.80059999999999898</v>
-      </c>
-      <c r="R9" s="7">
-        <v>0.78890000000000005</v>
-      </c>
-      <c r="S9" s="8">
-        <v>0.77159999999999895</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
-      <c r="B10">
-        <v>100</v>
-      </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="13">
-        <v>0.84589999999999899</v>
-      </c>
-      <c r="M10" s="14">
-        <v>0.84750000000000003</v>
-      </c>
-      <c r="N10" s="14">
-        <v>0.84350000000000003</v>
-      </c>
-      <c r="O10" s="14">
-        <v>0.83399999999999896</v>
-      </c>
-      <c r="P10" s="14">
-        <v>0.82350000000000001</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
-      <c r="B11">
-        <v>200</v>
-      </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="13">
-        <v>0.85550000000000004</v>
-      </c>
-      <c r="M11" s="14">
-        <v>0.85360000000000003</v>
-      </c>
-      <c r="N11" s="14">
-        <v>0.84640000000000004</v>
-      </c>
-      <c r="O11" s="14">
-        <v>0.83720000000000006</v>
-      </c>
-      <c r="P11" s="14">
-        <v>0.82720000000000005</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12">
-        <v>1000</v>
-      </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="15">
-        <v>0.86209999999999898</v>
-      </c>
-      <c r="M12" s="16">
-        <v>0.85840000000000005</v>
-      </c>
-      <c r="N12" s="16">
-        <v>0.85140000000000005</v>
-      </c>
-      <c r="O12" s="16">
-        <v>0.84079999999999899</v>
-      </c>
-      <c r="P12" s="16">
-        <v>0.82750000000000001</v>
-      </c>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="18"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="28">
-        <v>10</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="7">
-        <v>0.73199999999999898</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0.77090000000000003</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0.77680000000000005</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="53"/>
-      <c r="B19" s="28">
-        <v>100</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7">
-        <v>0.84809999999999897</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0.84809999999999897</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0.84589999999999899</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0.83799999999999897</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0.82589999999999897</v>
-      </c>
-      <c r="I19" s="7">
-        <v>0.81159999999999899</v>
-      </c>
-      <c r="J19" s="7">
-        <v>0.80489999999999895</v>
-      </c>
-      <c r="K19" s="7">
-        <v>0.79469999999999896</v>
-      </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
-      <c r="B20" s="29">
-        <v>200</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7">
-        <v>0.85570000000000002</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0.85570000000000002</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0.85550000000000004</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="7">
-        <v>0.81669999999999898</v>
-      </c>
-      <c r="J20" s="7">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="K20" s="7">
-        <v>0.79320000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="53"/>
-      <c r="B21" s="29">
-        <v>500</v>
-      </c>
-      <c r="C21" s="7">
-        <v>0.86209999999999898</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0.86209999999999898</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0.86209999999999898</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0.85999999999999899</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="53"/>
-      <c r="B22" s="30">
-        <v>1000</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.86229999999999896</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.86229999999999896</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="53"/>
-      <c r="B23" s="30">
-        <v>2000</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0.86439999999999895</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0.86439999999999895</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="53"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
+      <c r="I15" s="25">
+        <v>26</v>
+      </c>
+      <c r="J15" s="25">
+        <v>31</v>
+      </c>
+      <c r="K15" s="25">
+        <v>57</v>
+      </c>
+      <c r="L15" s="25">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C1:S1"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="C9:G12"/>
-    <mergeCell ref="L2:S2"/>
+  <mergeCells count="3">
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="A4:B5"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:J8 H9:J9 C9">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4:S8 Q9:S9">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:P12">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P13:S13 L4:S12">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9:J12 C4:J8 C13:J13 C9">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:S12">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18:K18 G19:K20">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18:K20 E21:K21">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:K25">
+  <conditionalFormatting sqref="D6:L6 C15:K15 C14:J14 L14 C13:I13 K13:L13 C12:H12 J12:L12 C11:G11 I11:L11 C10:F10 H10:L10 C9:E9 G9:L9 C8:D8 F8:L8 C7 E7:L7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2041,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2100,39 +1827,39 @@
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="80"/>
       <c r="B2" s="80"/>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="73"/>
-      <c r="M2" s="71" t="s">
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
+      <c r="M2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="73"/>
-      <c r="W2" s="71" t="s">
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="74"/>
+      <c r="W2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="74"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C3" s="37">
@@ -2219,7 +1946,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="37">
@@ -2252,7 +1979,7 @@
       <c r="K4" s="77">
         <v>1</v>
       </c>
-      <c r="L4" s="49"/>
+      <c r="L4" s="50"/>
       <c r="M4" s="77">
         <v>0.39979999999999899</v>
       </c>
@@ -2310,7 +2037,7 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="37">
         <v>4</v>
       </c>
@@ -2341,7 +2068,7 @@
       <c r="K5" s="77">
         <v>1</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="50"/>
       <c r="M5" s="77">
         <v>0.40110000000000001</v>
       </c>
@@ -2399,7 +2126,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="37">
         <v>6</v>
       </c>
@@ -2430,7 +2157,7 @@
       <c r="K6" s="77">
         <v>0.99992499999999895</v>
       </c>
-      <c r="L6" s="49"/>
+      <c r="L6" s="50"/>
       <c r="M6" s="77">
         <v>0.39839999999999898</v>
       </c>
@@ -2488,7 +2215,7 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7" s="64"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="37">
         <v>8</v>
       </c>
@@ -2519,7 +2246,7 @@
       <c r="K7" s="77">
         <v>0.99980000000000002</v>
       </c>
-      <c r="L7" s="49"/>
+      <c r="L7" s="50"/>
       <c r="M7" s="77">
         <v>0.39860000000000001</v>
       </c>
@@ -2583,25 +2310,25 @@
       <c r="X8" s="35"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
       <c r="U9" s="35"/>
       <c r="V9" s="35"/>
       <c r="W9" s="35"/>
       <c r="X9" s="35"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="82" t="s">
+      <c r="D10" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="82" t="s">
+      <c r="E10" s="83" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="37" t="s">
@@ -2613,16 +2340,16 @@
       <c r="X10" s="35"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C11" s="82">
+      <c r="C11" s="83">
         <v>4</v>
       </c>
-      <c r="D11" s="82">
+      <c r="D11" s="83">
         <v>128</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="83">
         <v>100</v>
       </c>
-      <c r="F11" s="83">
+      <c r="F11" s="84">
         <v>0.44350000000000001</v>
       </c>
     </row>
@@ -2754,53 +2481,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="I1" s="66" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="I1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="O1" s="66" t="s">
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="O1" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="I2" s="65" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="I2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="O2" s="65" t="s">
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="O2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C3" s="37">
@@ -2851,7 +2578,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="37">
@@ -2906,7 +2633,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="37">
         <v>4</v>
       </c>
@@ -2958,7 +2685,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="37">
         <v>6</v>
       </c>
@@ -3010,7 +2737,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="64"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="37">
         <v>8</v>
       </c>
@@ -3134,78 +2861,80 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L27" sqref="B17:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.1640625" customWidth="1"/>
+    <col min="1" max="2" width="8.1640625" customWidth="1"/>
+    <col min="3" max="12" width="8.6640625" customWidth="1"/>
+    <col min="13" max="25" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="51" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="45"/>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="Q2" s="70" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="Q2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73"/>
-      <c r="K3" s="65" t="s">
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74"/>
+      <c r="K3" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
       <c r="P3" s="35"/>
-      <c r="S3" s="65" t="s">
+      <c r="S3" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C4" s="37">
@@ -3256,7 +2985,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="68" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="37">
@@ -3277,7 +3006,7 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="68" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="37">
@@ -3299,7 +3028,7 @@
         <v>0.56020000000000003</v>
       </c>
       <c r="P5" s="35"/>
-      <c r="Q5" s="67" t="s">
+      <c r="Q5" s="68" t="s">
         <v>18</v>
       </c>
       <c r="R5" s="37">
@@ -3322,7 +3051,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="37">
         <v>4</v>
       </c>
@@ -3341,7 +3070,7 @@
       <c r="G6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="67"/>
+      <c r="I6" s="68"/>
       <c r="J6" s="37">
         <v>4</v>
       </c>
@@ -3360,7 +3089,7 @@
       <c r="O6" s="2">
         <v>0.55220000000000002</v>
       </c>
-      <c r="Q6" s="67"/>
+      <c r="Q6" s="68"/>
       <c r="R6" s="37">
         <v>4</v>
       </c>
@@ -3381,7 +3110,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="37">
         <v>6</v>
       </c>
@@ -3400,7 +3129,7 @@
       <c r="G7" s="2">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I7" s="67"/>
+      <c r="I7" s="68"/>
       <c r="J7" s="37">
         <v>6</v>
       </c>
@@ -3419,7 +3148,7 @@
       <c r="O7" s="2">
         <v>0.55489999999999895</v>
       </c>
-      <c r="Q7" s="67"/>
+      <c r="Q7" s="68"/>
       <c r="R7" s="37">
         <v>6</v>
       </c>
@@ -3440,7 +3169,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="37">
         <v>8</v>
       </c>
@@ -3459,7 +3188,7 @@
       <c r="G8" s="2">
         <v>0.99975000000000003</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="68"/>
       <c r="J8" s="37">
         <v>8</v>
       </c>
@@ -3478,7 +3207,7 @@
       <c r="O8" s="2">
         <v>0.55279999999999896</v>
       </c>
-      <c r="Q8" s="67"/>
+      <c r="Q8" s="68"/>
       <c r="R8" s="37">
         <v>8</v>
       </c>
@@ -3499,7 +3228,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="37">
         <v>10</v>
       </c>
@@ -3518,7 +3247,7 @@
       <c r="G9" s="2">
         <v>0.99929999999999897</v>
       </c>
-      <c r="I9" s="67"/>
+      <c r="I9" s="68"/>
       <c r="J9" s="37">
         <v>10</v>
       </c>
@@ -3537,7 +3266,7 @@
       <c r="O9" s="2">
         <v>0.55059999999999898</v>
       </c>
-      <c r="Q9" s="67"/>
+      <c r="Q9" s="68"/>
       <c r="R9" s="37">
         <v>10</v>
       </c>
@@ -3557,10 +3286,7 @@
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="349" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="M33" s="35"/>
       <c r="N33" s="35"/>
@@ -3586,27 +3312,27 @@
       <c r="A36" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="C36" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
       <c r="J36" s="41"/>
       <c r="K36" s="41"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="65" t="s">
+      <c r="M36" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
-      <c r="P36" s="65"/>
-      <c r="Q36" s="65"/>
-      <c r="R36" s="65"/>
-      <c r="S36" s="65"/>
+      <c r="N36" s="66"/>
+      <c r="O36" s="66"/>
+      <c r="P36" s="66"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="66"/>
+      <c r="S36" s="66"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C37" s="38">
@@ -3656,7 +3382,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="68" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="37">
@@ -3711,7 +3437,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="67"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="37">
         <v>100</v>
       </c>
@@ -3764,7 +3490,7 @@
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="67"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="37">
         <v>300</v>
       </c>
@@ -3817,7 +3543,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="67"/>
+      <c r="A41" s="68"/>
       <c r="B41" s="39">
         <v>500</v>
       </c>
@@ -3864,7 +3590,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A42" s="67"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="39">
         <v>1000</v>
       </c>
@@ -3911,7 +3637,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="67"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="37"/>
       <c r="C43" s="36"/>
       <c r="D43" s="36"/>
@@ -3934,18 +3660,18 @@
       <c r="A45" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="M45" s="69" t="s">
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="M45" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="N45" s="69"/>
-      <c r="O45" s="69"/>
-      <c r="P45" s="69"/>
+      <c r="N45" s="70"/>
+      <c r="O45" s="70"/>
+      <c r="P45" s="70"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C46" s="37">
@@ -3974,7 +3700,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A47" s="68" t="s">
+      <c r="A47" s="69" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="37">
@@ -4014,7 +3740,7 @@
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A48" s="68"/>
+      <c r="A48" s="69"/>
       <c r="B48" s="37">
         <v>4</v>
       </c>
@@ -4052,7 +3778,7 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="68"/>
+      <c r="A49" s="69"/>
       <c r="B49" s="37">
         <v>8</v>
       </c>
@@ -4090,7 +3816,7 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" s="68"/>
+      <c r="A50" s="69"/>
       <c r="B50" s="37">
         <v>16</v>
       </c>
@@ -4131,20 +3857,20 @@
       <c r="A52" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="69" t="s">
+      <c r="D52" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="69"/>
-      <c r="N52" s="69" t="s">
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="N52" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="O52" s="69"/>
-      <c r="P52" s="69"/>
-      <c r="Q52" s="69"/>
-      <c r="R52" s="69"/>
+      <c r="O52" s="70"/>
+      <c r="P52" s="70"/>
+      <c r="Q52" s="70"/>
+      <c r="R52" s="70"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C53" s="44"/>
@@ -4181,7 +3907,7 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="68" t="s">
+      <c r="A54" s="69" t="s">
         <v>18</v>
       </c>
       <c r="B54" s="37">
@@ -4227,7 +3953,7 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="68"/>
+      <c r="A55" s="69"/>
       <c r="B55" s="37">
         <v>4</v>
       </c>
@@ -4271,7 +3997,7 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="68"/>
+      <c r="A56" s="69"/>
       <c r="B56" s="37">
         <v>8</v>
       </c>
@@ -4315,7 +4041,7 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="68"/>
+      <c r="A57" s="69"/>
       <c r="B57" s="37">
         <v>16</v>
       </c>
@@ -4380,7 +4106,7 @@
     <mergeCell ref="A47:A50"/>
   </mergeCells>
   <conditionalFormatting sqref="P3:P5">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4392,7 +4118,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:G9">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4404,7 +4130,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5:W9">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4416,7 +4142,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43:S43">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4428,7 +4154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M40:S42">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4440,7 +4166,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M47:P50">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4452,7 +4178,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:P57">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4464,7 +4190,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N54:R57">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4476,7 +4202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33:Q35">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4488,7 +4214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:O9">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4526,62 +4252,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="51" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="I2" s="74" t="s">
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="I2" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="P2" s="74" t="s">
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="P2" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="J3" s="65" t="s">
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="J3" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="Q3" s="65" t="s">
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="Q3" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C4" s="38">
@@ -4593,10 +4319,10 @@
       <c r="E4" s="38">
         <v>3</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="52">
         <v>4</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="52">
         <v>8</v>
       </c>
       <c r="J4" s="38">
@@ -4608,10 +4334,10 @@
       <c r="L4" s="38">
         <v>3</v>
       </c>
-      <c r="M4" s="51">
+      <c r="M4" s="52">
         <v>4</v>
       </c>
-      <c r="N4" s="51">
+      <c r="N4" s="52">
         <v>8</v>
       </c>
       <c r="Q4" s="38">
@@ -4623,424 +4349,424 @@
       <c r="S4" s="38">
         <v>3</v>
       </c>
-      <c r="T4" s="51">
+      <c r="T4" s="52">
         <v>4</v>
       </c>
-      <c r="U4" s="51">
+      <c r="U4" s="52">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="63" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="37">
         <v>24</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="50">
         <v>0.94674999999999898</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="50">
         <v>0.93752500000000005</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="50">
         <v>0.93232499999999896</v>
       </c>
-      <c r="F5" s="49">
+      <c r="F5" s="50">
         <v>0.92849999999999899</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="50">
         <v>0.92422499999999896</v>
       </c>
       <c r="I5" s="37">
         <v>24</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="50">
         <v>0.30740000000000001</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="50">
         <v>0.30980000000000002</v>
       </c>
-      <c r="L5" s="49">
+      <c r="L5" s="50">
         <v>0.30730000000000002</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="50">
         <v>0.30470000000000003</v>
       </c>
-      <c r="N5" s="49">
+      <c r="N5" s="50">
         <v>0.29339999999999899</v>
       </c>
       <c r="P5" s="37">
         <v>24</v>
       </c>
-      <c r="Q5" s="49">
+      <c r="Q5" s="50">
         <v>0.294899999999999</v>
       </c>
-      <c r="R5" s="49">
+      <c r="R5" s="50">
         <v>0.29977500000000001</v>
       </c>
-      <c r="S5" s="49">
+      <c r="S5" s="50">
         <v>0.29970000000000002</v>
       </c>
-      <c r="T5" s="49">
+      <c r="T5" s="50">
         <v>0.29604999999999898</v>
       </c>
-      <c r="U5" s="49">
+      <c r="U5" s="50">
         <v>0.29647499999999899</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="37">
         <v>28</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="50">
         <v>0.92659999999999898</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="50">
         <v>0.914349999999999</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="50">
         <v>0.90785000000000005</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="50">
         <v>0.90387499999999898</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="50">
         <v>0.89637500000000003</v>
       </c>
       <c r="I6" s="37">
         <v>28</v>
       </c>
-      <c r="J6" s="49">
+      <c r="J6" s="50">
         <v>0.30959999999999899</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="50">
         <v>0.30349999999999899</v>
       </c>
-      <c r="L6" s="49">
+      <c r="L6" s="50">
         <v>0.30520000000000003</v>
       </c>
-      <c r="M6" s="49">
+      <c r="M6" s="50">
         <v>0.30009999999999898</v>
       </c>
-      <c r="N6" s="49">
+      <c r="N6" s="50">
         <v>0.2923</v>
       </c>
       <c r="P6" s="37">
         <v>28</v>
       </c>
-      <c r="Q6" s="49">
+      <c r="Q6" s="50">
         <v>0.29752499999999898</v>
       </c>
-      <c r="R6" s="49">
+      <c r="R6" s="50">
         <v>0.29897499999999899</v>
       </c>
-      <c r="S6" s="49">
+      <c r="S6" s="50">
         <v>0.29965000000000003</v>
       </c>
-      <c r="T6" s="49">
+      <c r="T6" s="50">
         <v>0.30117500000000003</v>
       </c>
-      <c r="U6" s="49">
+      <c r="U6" s="50">
         <v>0.29652499999999898</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="37">
         <v>32</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="50">
         <v>0.90502499999999897</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="50">
         <v>0.890674999999999</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="50">
         <v>0.88380000000000003</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="50">
         <v>0.87860000000000005</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="50">
         <v>0.86807500000000004</v>
       </c>
       <c r="I7" s="37">
         <v>32</v>
       </c>
-      <c r="J7" s="49">
+      <c r="J7" s="50">
         <v>0.311499999999999</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="50">
         <v>0.30620000000000003</v>
       </c>
-      <c r="L7" s="49">
+      <c r="L7" s="50">
         <v>0.30380000000000001</v>
       </c>
-      <c r="M7" s="49">
+      <c r="M7" s="50">
         <v>0.30320000000000003</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="50">
         <v>0.2923</v>
       </c>
       <c r="P7" s="37">
         <v>32</v>
       </c>
-      <c r="Q7" s="49">
+      <c r="Q7" s="50">
         <v>0.302449999999999</v>
       </c>
-      <c r="R7" s="49">
+      <c r="R7" s="50">
         <v>0.302974999999999</v>
       </c>
-      <c r="S7" s="49">
+      <c r="S7" s="50">
         <v>0.29997499999999899</v>
       </c>
-      <c r="T7" s="49">
+      <c r="T7" s="50">
         <v>0.30109999999999898</v>
       </c>
-      <c r="U7" s="49">
+      <c r="U7" s="50">
         <v>0.29512500000000003</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="37">
         <v>40</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="50">
         <v>0.86412500000000003</v>
       </c>
-      <c r="D8" s="49">
+      <c r="D8" s="50">
         <v>0.84560000000000002</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="50">
         <v>0.83809999999999896</v>
       </c>
-      <c r="F8" s="49">
+      <c r="F8" s="50">
         <v>0.82920000000000005</v>
       </c>
-      <c r="G8" s="49">
+      <c r="G8" s="50">
         <v>0.81620000000000004</v>
       </c>
       <c r="I8" s="37">
         <v>40</v>
       </c>
-      <c r="J8" s="49">
+      <c r="J8" s="50">
         <v>0.3049</v>
       </c>
-      <c r="K8" s="49">
+      <c r="K8" s="50">
         <v>0.3054</v>
       </c>
-      <c r="L8" s="49">
+      <c r="L8" s="50">
         <v>0.306999999999999</v>
       </c>
-      <c r="M8" s="49">
+      <c r="M8" s="50">
         <v>0.29980000000000001</v>
       </c>
-      <c r="N8" s="49">
+      <c r="N8" s="50">
         <v>0.29020000000000001</v>
       </c>
       <c r="P8" s="37">
         <v>40</v>
       </c>
-      <c r="Q8" s="49">
+      <c r="Q8" s="50">
         <v>0.29794999999999899</v>
       </c>
-      <c r="R8" s="49">
+      <c r="R8" s="50">
         <v>0.29982500000000001</v>
       </c>
-      <c r="S8" s="49">
+      <c r="S8" s="50">
         <v>0.30247499999999899</v>
       </c>
-      <c r="T8" s="49">
+      <c r="T8" s="50">
         <v>0.29877500000000001</v>
       </c>
-      <c r="U8" s="49">
+      <c r="U8" s="50">
         <v>0.29585</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="37">
         <v>48</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="50">
         <v>0.822075</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="50">
         <v>0.80464999999999898</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="50">
         <v>0.79227499999999895</v>
       </c>
-      <c r="F9" s="49">
+      <c r="F9" s="50">
         <v>0.78510000000000002</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="50">
         <v>0.76924999999999899</v>
       </c>
       <c r="I9" s="37">
         <v>48</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="50">
         <v>0.30919999999999898</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="50">
         <v>0.30449999999999899</v>
       </c>
-      <c r="L9" s="49">
+      <c r="L9" s="50">
         <v>0.30630000000000002</v>
       </c>
-      <c r="M9" s="49">
+      <c r="M9" s="50">
         <v>0.29509999999999897</v>
       </c>
-      <c r="N9" s="49">
+      <c r="N9" s="50">
         <v>0.29399999999999898</v>
       </c>
       <c r="P9" s="37">
         <v>48</v>
       </c>
-      <c r="Q9" s="49">
+      <c r="Q9" s="50">
         <v>0.30047499999999899</v>
       </c>
-      <c r="R9" s="49">
+      <c r="R9" s="50">
         <v>0.30312499999999898</v>
       </c>
-      <c r="S9" s="49">
+      <c r="S9" s="50">
         <v>0.30112499999999898</v>
       </c>
-      <c r="T9" s="49">
+      <c r="T9" s="50">
         <v>0.30102499999999899</v>
       </c>
-      <c r="U9" s="49">
+      <c r="U9" s="50">
         <v>0.29454999999999898</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="39">
         <v>64</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="50">
         <v>0.75567499999999899</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="50">
         <v>0.735424999999999</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="50">
         <v>0.72297500000000003</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="50">
         <v>0.71287500000000004</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="50">
         <v>0.69272500000000004</v>
       </c>
-      <c r="H10" s="49"/>
+      <c r="H10" s="50"/>
       <c r="I10" s="39">
         <v>64</v>
       </c>
-      <c r="J10" s="49">
+      <c r="J10" s="50">
         <v>0.30630000000000002</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="50">
         <v>0.30719999999999897</v>
       </c>
-      <c r="L10" s="49">
+      <c r="L10" s="50">
         <v>0.30080000000000001</v>
       </c>
-      <c r="M10" s="49">
+      <c r="M10" s="50">
         <v>0.297399999999999</v>
       </c>
-      <c r="N10" s="49">
+      <c r="N10" s="50">
         <v>0.28839999999999899</v>
       </c>
-      <c r="O10" s="49"/>
+      <c r="O10" s="50"/>
       <c r="P10" s="39">
         <v>64</v>
       </c>
-      <c r="Q10" s="49">
+      <c r="Q10" s="50">
         <v>0.29859999999999898</v>
       </c>
-      <c r="R10" s="49">
+      <c r="R10" s="50">
         <v>0.30135000000000001</v>
       </c>
-      <c r="S10" s="49">
+      <c r="S10" s="50">
         <v>0.30064999999999897</v>
       </c>
-      <c r="T10" s="49">
+      <c r="T10" s="50">
         <v>0.29857499999999898</v>
       </c>
-      <c r="U10" s="49">
+      <c r="U10" s="50">
         <v>0.29202499999999898</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="64"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="39">
         <v>128</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="50">
         <v>0.59212500000000001</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="50">
         <v>0.57387500000000002</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="50">
         <v>0.55977500000000002</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="50">
         <v>0.55012499999999898</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="50">
         <v>0.52577499999999899</v>
       </c>
-      <c r="H11" s="49"/>
+      <c r="H11" s="50"/>
       <c r="I11" s="39">
         <v>128</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="50">
         <v>0.3049</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="50">
         <v>0.30349999999999899</v>
       </c>
-      <c r="L11" s="49">
+      <c r="L11" s="50">
         <v>0.29480000000000001</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="50">
         <v>0.29360000000000003</v>
       </c>
-      <c r="N11" s="49">
+      <c r="N11" s="50">
         <v>0.285299999999999</v>
       </c>
-      <c r="O11" s="49"/>
+      <c r="O11" s="50"/>
       <c r="P11" s="39">
         <v>128</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="50">
         <v>0.299924999999999</v>
       </c>
-      <c r="R11" s="49">
+      <c r="R11" s="50">
         <v>0.29970000000000002</v>
       </c>
-      <c r="S11" s="49">
+      <c r="S11" s="50">
         <v>0.29997499999999899</v>
       </c>
-      <c r="T11" s="49">
+      <c r="T11" s="50">
         <v>0.29512500000000003</v>
       </c>
-      <c r="U11" s="49">
+      <c r="U11" s="50">
         <v>0.29110000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5146,7 +4872,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5158,45 +4884,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="K1" s="66" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="K1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C3" s="37">
@@ -5244,7 +4970,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="68" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="37">
@@ -5294,7 +5020,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="37">
         <v>100</v>
       </c>
@@ -5342,7 +5068,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="37">
         <v>200</v>
       </c>
@@ -5390,7 +5116,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="37">
         <v>500</v>
       </c>
@@ -5438,7 +5164,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="37">
         <v>1000</v>
       </c>
@@ -5486,7 +5212,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="37">
         <v>2000</v>
       </c>
@@ -5533,13 +5259,16 @@
         <v>0.50929999999999898</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="76" t="s">
+    <row r="11" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5564,4 +5293,871 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="9" width="8.1640625" customWidth="1"/>
+    <col min="10" max="13" width="7.83203125" customWidth="1"/>
+    <col min="14" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="19" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="57"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C3" s="22">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23">
+        <v>4</v>
+      </c>
+      <c r="E3" s="23">
+        <v>8</v>
+      </c>
+      <c r="F3" s="23">
+        <v>16</v>
+      </c>
+      <c r="G3" s="23">
+        <v>32</v>
+      </c>
+      <c r="H3" s="23">
+        <v>64</v>
+      </c>
+      <c r="I3" s="23">
+        <v>128</v>
+      </c>
+      <c r="J3" s="24">
+        <v>256</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="22">
+        <v>2</v>
+      </c>
+      <c r="M3" s="23">
+        <v>4</v>
+      </c>
+      <c r="N3" s="23">
+        <v>8</v>
+      </c>
+      <c r="O3" s="23">
+        <v>16</v>
+      </c>
+      <c r="P3" s="23">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>64</v>
+      </c>
+      <c r="R3" s="23">
+        <v>128</v>
+      </c>
+      <c r="S3" s="24">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7">
+        <v>0.85303333333333298</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.86468333333333303</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.86431666666666596</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.86809999999999898</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="7">
+        <v>0.60880000000000001</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>0.63260000000000005</v>
+      </c>
+      <c r="R4" s="7">
+        <v>0.633099999999999</v>
+      </c>
+      <c r="S4" s="8">
+        <v>0.64539999999999897</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="54"/>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7">
+        <v>0.85394999999999899</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.86486666666666601</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.86548333333333305</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.86916666666666598</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="7">
+        <v>0.60140000000000005</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>0.62539999999999896</v>
+      </c>
+      <c r="R5" s="7">
+        <v>0.63380000000000003</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0.637099999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7">
+        <v>0.97594999999999898</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.97423333333333295</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.97135000000000005</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.96968333333333301</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="7">
+        <v>0.72030000000000005</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>0.72250000000000003</v>
+      </c>
+      <c r="R6" s="7">
+        <v>0.72250000000000003</v>
+      </c>
+      <c r="S6" s="8">
+        <v>0.71379999999999899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7">
+        <v>0.99546666666666594</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.99460000000000004</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.99273333333333302</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.99099999999999899</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="7">
+        <v>0.7671</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>0.76559999999999895</v>
+      </c>
+      <c r="R7" s="7">
+        <v>0.75509999999999899</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0.74829999999999897</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7">
+        <v>0.99944999999999895</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.99928333333333297</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.99861666666666604</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.99804999999999899</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="7">
+        <v>0.79859999999999898</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>0.78459999999999896</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0.77629999999999899</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0.76370000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" s="59">
+        <v>0.999966666666666</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="7">
+        <v>0.999966666666666</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.99978333333333302</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="13">
+        <v>0.83620000000000005</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0.83309999999999895</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0.83640000000000003</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0.82730000000000004</v>
+      </c>
+      <c r="P9" s="14">
+        <v>0.81630000000000003</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>0.80059999999999898</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0.78890000000000005</v>
+      </c>
+      <c r="S9" s="8">
+        <v>0.77159999999999895</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="54"/>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="13">
+        <v>0.84589999999999899</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0.84350000000000003</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0.83399999999999896</v>
+      </c>
+      <c r="P10" s="14">
+        <v>0.82350000000000001</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="54"/>
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="13">
+        <v>0.85550000000000004</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0.85360000000000003</v>
+      </c>
+      <c r="N11" s="14">
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="P11" s="14">
+        <v>0.82720000000000005</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="15">
+        <v>0.86209999999999898</v>
+      </c>
+      <c r="M12" s="16">
+        <v>0.85840000000000005</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0.85140000000000005</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0.84079999999999899</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="18"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="28">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="7">
+        <v>0.73199999999999898</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0.77090000000000003</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.77680000000000005</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="54"/>
+      <c r="B19" s="28">
+        <v>100</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7">
+        <v>0.84809999999999897</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.84809999999999897</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.84589999999999899</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.83799999999999897</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.82589999999999897</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.81159999999999899</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0.80489999999999895</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0.79469999999999896</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="54"/>
+      <c r="B20" s="29">
+        <v>200</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7">
+        <v>0.85570000000000002</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.85570000000000002</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.85550000000000004</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="7">
+        <v>0.81669999999999898</v>
+      </c>
+      <c r="J20" s="7">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0.79320000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="54"/>
+      <c r="B21" s="29">
+        <v>500</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.86209999999999898</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.86209999999999898</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.86209999999999898</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.85999999999999899</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="54"/>
+      <c r="B22" s="30">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.86229999999999896</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.86229999999999896</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="54"/>
+      <c r="B23" s="30">
+        <v>2000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.86439999999999895</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0.86439999999999895</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="54"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="54"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+    </row>
+    <row r="27" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C1:S1"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="C9:G12"/>
+    <mergeCell ref="L2:S2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G4:J8 H9:J9 C9">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:S8 Q9:S9">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:P12">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13:S13 L4:S12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:J12 C4:J8 C13:J13 C9">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:S12">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:K18 G19:K20">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:K20 E21:K21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:K25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change color conf mat
</commit_message>
<xml_diff>
--- a/resultats/random_forest_gridsearch.xlsx
+++ b/resultats/random_forest_gridsearch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="860" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BEST" sheetId="8" r:id="rId1"/>
@@ -91,7 +91,7 @@
     </textPr>
   </connection>
   <connection id="2" name="confusion_rf1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/confusion_rf.csv" thousands=" " space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/confusion_rf.csv" thousands=" " space="1" consecutive="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -172,7 +172,7 @@
     </textPr>
   </connection>
   <connection id="10" name="gridsearch_accuracy_oob7" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -186,7 +186,7 @@
     </textPr>
   </connection>
   <connection id="11" name="gridsearch_accuracy_oob8" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_oob.csv" thousands=" ">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -217,7 +217,7 @@
     </textPr>
   </connection>
   <connection id="14" name="gridsearch_accuracy_test11" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -231,7 +231,7 @@
     </textPr>
   </connection>
   <connection id="15" name="gridsearch_accuracy_test12" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -304,7 +304,7 @@
     </textPr>
   </connection>
   <connection id="23" name="gridsearch_accuracy_test9" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_test.csv" thousands=" ">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -335,7 +335,7 @@
     </textPr>
   </connection>
   <connection id="26" name="gridsearch_accuracy_train10" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields>
         <textField/>
       </textFields>
@@ -399,7 +399,7 @@
     </textPr>
   </connection>
   <connection id="33" name="gridsearch_accuracy_train8" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -413,7 +413,7 @@
     </textPr>
   </connection>
   <connection id="34" name="gridsearch_accuracy_train9" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch_accuracy_train.csv" thousands=" ">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -1218,23 +1218,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1245,6 +1250,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1254,10 +1265,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1296,20 +1310,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
@@ -1338,11 +1338,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion_rf_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion_rf" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1354,7 +1354,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1362,11 +1362,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1374,15 +1374,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion_rf" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion_rf_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1390,23 +1390,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_2" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_3" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_3" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1414,43 +1414,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_3" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob_3" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_2" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1458,11 +1458,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train_1" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test_1" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_train" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1470,7 +1470,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_oob" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_accuracy_test" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1749,26 +1749,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68">
         <v>0.57889999999999997</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
@@ -1787,26 +1787,26 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="63" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="47" t="s">
         <v>36</v>
       </c>
@@ -1839,13 +1839,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="71" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="89">
+      <c r="C7" s="63">
         <v>627</v>
       </c>
       <c r="D7" s="25">
@@ -1877,14 +1877,14 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="64"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="57" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="25">
         <v>41</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="63">
         <v>720</v>
       </c>
       <c r="E8" s="25">
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="57" t="s">
         <v>38</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="D9" s="25">
         <v>30</v>
       </c>
-      <c r="E9" s="89">
+      <c r="E9" s="63">
         <v>352</v>
       </c>
       <c r="F9" s="25">
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="64"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="57" t="s">
         <v>39</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="E10" s="25">
         <v>36</v>
       </c>
-      <c r="F10" s="89">
+      <c r="F10" s="63">
         <v>445</v>
       </c>
       <c r="G10" s="25">
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="64"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="57" t="s">
         <v>40</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="F11" s="25">
         <v>99</v>
       </c>
-      <c r="G11" s="89">
+      <c r="G11" s="63">
         <v>456</v>
       </c>
       <c r="H11" s="25">
@@ -2021,7 +2021,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="64"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="57" t="s">
         <v>41</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="G12" s="25">
         <v>58</v>
       </c>
-      <c r="H12" s="89">
+      <c r="H12" s="63">
         <v>458</v>
       </c>
       <c r="I12" s="25">
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="64"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="57" t="s">
         <v>42</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="H13" s="25">
         <v>43</v>
       </c>
-      <c r="I13" s="89">
+      <c r="I13" s="63">
         <v>720</v>
       </c>
       <c r="J13" s="25">
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="64"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="57" t="s">
         <v>43</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="I14" s="25">
         <v>33</v>
       </c>
-      <c r="J14" s="89">
+      <c r="J14" s="63">
         <v>619</v>
       </c>
       <c r="K14" s="25">
@@ -2129,7 +2129,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="64"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="57" t="s">
         <v>44</v>
       </c>
@@ -2157,7 +2157,7 @@
       <c r="J15" s="25">
         <v>13</v>
       </c>
-      <c r="K15" s="89">
+      <c r="K15" s="63">
         <v>703</v>
       </c>
       <c r="L15" s="25">
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="64"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="57" t="s">
         <v>45</v>
       </c>
@@ -2196,7 +2196,7 @@
       <c r="K16" s="25">
         <v>57</v>
       </c>
-      <c r="L16" s="89">
+      <c r="L16" s="63">
         <v>689</v>
       </c>
     </row>
@@ -2207,26 +2207,26 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="94">
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68">
         <v>0.97550000000000003</v>
       </c>
-      <c r="F20" s="93" t="s">
+      <c r="F20" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93" t="s">
+      <c r="G20" s="67"/>
+      <c r="H20" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
@@ -2249,26 +2249,26 @@
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="63" t="s">
+      <c r="B24" s="73"/>
+      <c r="C24" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="65"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
       <c r="C25" s="51">
         <v>0</v>
       </c>
@@ -2301,13 +2301,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="71" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="51">
         <v>0</v>
       </c>
-      <c r="C26" s="89">
+      <c r="C26" s="63">
         <v>972</v>
       </c>
       <c r="D26" s="25">
@@ -2339,14 +2339,14 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="64"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="51">
         <v>1</v>
       </c>
       <c r="C27" s="25">
         <v>0</v>
       </c>
-      <c r="D27" s="89">
+      <c r="D27" s="63">
         <v>1127</v>
       </c>
       <c r="E27" s="25">
@@ -2375,7 +2375,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="64"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="51">
         <v>2</v>
       </c>
@@ -2385,7 +2385,7 @@
       <c r="D28" s="25">
         <v>1</v>
       </c>
-      <c r="E28" s="89">
+      <c r="E28" s="63">
         <v>1014</v>
       </c>
       <c r="F28" s="25">
@@ -2411,7 +2411,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="64"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="51">
         <v>3</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="E29" s="25">
         <v>7</v>
       </c>
-      <c r="F29" s="89">
+      <c r="F29" s="63">
         <v>981</v>
       </c>
       <c r="G29" s="25">
@@ -2447,7 +2447,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="64"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="51">
         <v>4</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="F30" s="25">
         <v>0</v>
       </c>
-      <c r="G30" s="89">
+      <c r="G30" s="63">
         <v>958</v>
       </c>
       <c r="H30" s="25">
@@ -2483,7 +2483,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="64"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="51">
         <v>5</v>
       </c>
@@ -2502,7 +2502,7 @@
       <c r="G31" s="25">
         <v>0</v>
       </c>
-      <c r="H31" s="89">
+      <c r="H31" s="63">
         <v>868</v>
       </c>
       <c r="I31" s="25">
@@ -2519,7 +2519,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="64"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="51">
         <v>6</v>
       </c>
@@ -2541,7 +2541,7 @@
       <c r="H32" s="25">
         <v>2</v>
       </c>
-      <c r="I32" s="89">
+      <c r="I32" s="63">
         <v>941</v>
       </c>
       <c r="J32" s="25">
@@ -2555,7 +2555,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="64"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="51">
         <v>7</v>
       </c>
@@ -2580,7 +2580,7 @@
       <c r="I33" s="25">
         <v>0</v>
       </c>
-      <c r="J33" s="89">
+      <c r="J33" s="63">
         <v>999</v>
       </c>
       <c r="K33" s="25">
@@ -2591,7 +2591,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="64"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="51">
         <v>8</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="J34" s="25">
         <v>6</v>
       </c>
-      <c r="K34" s="89">
+      <c r="K34" s="63">
         <v>934</v>
       </c>
       <c r="L34" s="25">
@@ -2627,7 +2627,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="64"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="51">
         <v>9</v>
       </c>
@@ -2658,7 +2658,7 @@
       <c r="K35" s="25">
         <v>3</v>
       </c>
-      <c r="L35" s="89">
+      <c r="L35" s="63">
         <v>961</v>
       </c>
     </row>
@@ -2672,7 +2672,7 @@
     <mergeCell ref="A24:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:L7 C16:K16 C15:J15 L15 C14:I14 K14:L14 C13:H13 J13:L13 C12:G12 I12:L12 C11:F11 H11:L11 C10:E10 G10:L10 C9:D9 F9:L9 C8 E8:L8">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2684,12 +2684,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:L26 C35:K35 C34:J34 L34 C33:I33 K33:L33 C32:H32 J32:L32 C31:G31 I31:L31 C30:F30 H30:L30 C29:E29 G29:L29 C28:D28 F28:L28 C27 E27:L27">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:L7 C16:K16 C15:J15 L15 C14:I14 K14:L14 C13:H13 J13:L13 C12:G12 I12:L12 C11:F11 H11:L11 C10:E10 G10:L10 C9:D9 F9:L9 C8 E8:L8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:L26 C35:K35 C34:J34 L34 C33:I33 K33:L33 C32:H32 J32:L32 C31:G31 I31:L31 C30:F30 H30:L30 C29:E29 G29:L29 C28:D28 F28:L28 C27 E27:L27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
@@ -2720,48 +2740,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="83"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="93"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="81" t="s">
+      <c r="L2" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="83"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="93"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C3" s="22">
@@ -2815,7 +2835,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="90" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -2856,7 +2876,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
+      <c r="A5" s="90"/>
       <c r="B5">
         <v>2</v>
       </c>
@@ -2895,7 +2915,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="80"/>
+      <c r="A6" s="90"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -2934,7 +2954,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="80"/>
+      <c r="A7" s="90"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -2973,7 +2993,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="80"/>
+      <c r="A8" s="90"/>
       <c r="B8">
         <v>20</v>
       </c>
@@ -3012,17 +3032,17 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
+      <c r="A9" s="90"/>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="95">
         <v>0.999966666666666</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
       <c r="H9" s="7">
         <v>0.999966666666666</v>
       </c>
@@ -3059,15 +3079,15 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="80"/>
+      <c r="A10" s="90"/>
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="10"/>
@@ -3092,15 +3112,15 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="80"/>
+      <c r="A11" s="90"/>
       <c r="B11">
         <v>200</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="10"/>
@@ -3125,15 +3145,15 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="80"/>
+      <c r="A12" s="90"/>
       <c r="B12">
         <v>1000</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="12"/>
@@ -3190,20 +3210,20 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="84" t="s">
+      <c r="A16" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="79" t="s">
+      <c r="B16" s="94"/>
+      <c r="C16" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
       <c r="K16" s="26"/>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
@@ -3215,8 +3235,8 @@
       <c r="S16" s="27"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="84"/>
-      <c r="B17" s="84"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="23" t="s">
         <v>13</v>
       </c>
@@ -3248,7 +3268,7 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="90" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="28">
@@ -3273,7 +3293,7 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="28">
         <v>100</v>
       </c>
@@ -3306,7 +3326,7 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="80"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="29">
         <v>200</v>
       </c>
@@ -3333,7 +3353,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="80"/>
+      <c r="A21" s="90"/>
       <c r="B21" s="29">
         <v>500</v>
       </c>
@@ -3356,7 +3376,7 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="80"/>
+      <c r="A22" s="90"/>
       <c r="B22" s="30">
         <v>1000</v>
       </c>
@@ -3375,7 +3395,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="80"/>
+      <c r="A23" s="90"/>
       <c r="B23" s="30">
         <v>2000</v>
       </c>
@@ -3394,7 +3414,7 @@
       <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="80"/>
+      <c r="A24" s="90"/>
       <c r="B24" s="33"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -3407,7 +3427,7 @@
       <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="80"/>
+      <c r="A25" s="90"/>
       <c r="B25" s="30"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -3589,77 +3609,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="N2" s="66" t="s">
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="N2" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="Y2" s="66" t="s">
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="Y2" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="N3" s="63" t="s">
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="N3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="Y3" s="63" t="s">
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="72"/>
+      <c r="Y3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
+      <c r="Z3" s="72"/>
+      <c r="AA3" s="72"/>
+      <c r="AB3" s="72"/>
+      <c r="AC3" s="72"/>
+      <c r="AD3" s="72"/>
+      <c r="AE3" s="72"/>
+      <c r="AF3" s="72"/>
+      <c r="AG3" s="72"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="C4" s="37">
@@ -3745,7 +3765,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="37">
@@ -3842,7 +3862,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="37">
         <v>2</v>
       </c>
@@ -3937,7 +3957,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="37">
         <v>4</v>
       </c>
@@ -4032,7 +4052,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="37">
         <v>8</v>
       </c>
@@ -4127,7 +4147,7 @@
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="37">
         <v>16</v>
       </c>
@@ -4553,7 +4573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -4580,68 +4600,68 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="19" x14ac:dyDescent="0.2">
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="M3" s="66" t="s">
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="M3" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="W3" s="66" t="s">
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="75"/>
+      <c r="W3" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="66"/>
-      <c r="Y3" s="66"/>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66"/>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="66"/>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="75"/>
+      <c r="AA3" s="75"/>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="75"/>
+      <c r="AD3" s="75"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="M4" s="63" t="s">
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="M4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
-      <c r="W4" s="63" t="s">
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="W4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="X4" s="63"/>
-      <c r="Y4" s="63"/>
-      <c r="Z4" s="63"/>
-      <c r="AA4" s="63"/>
-      <c r="AB4" s="63"/>
-      <c r="AC4" s="63"/>
-      <c r="AD4" s="63"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="72"/>
+      <c r="AD4" s="72"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C5" s="37">
@@ -4668,7 +4688,7 @@
       <c r="J5" s="37">
         <v>24</v>
       </c>
-      <c r="K5" s="90"/>
+      <c r="K5" s="64"/>
       <c r="M5" s="37">
         <v>1</v>
       </c>
@@ -4719,7 +4739,7 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="76" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="37">
@@ -4807,7 +4827,7 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="70"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="37">
         <v>2</v>
       </c>
@@ -4893,7 +4913,7 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="70"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="37">
         <v>4</v>
       </c>
@@ -4979,7 +4999,7 @@
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="37">
         <v>8</v>
       </c>
@@ -5065,7 +5085,7 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="37">
         <v>16</v>
       </c>
@@ -5206,7 +5226,7 @@
   <dimension ref="A1:AD12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5223,73 +5243,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="65" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="19" x14ac:dyDescent="0.2">
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="M2" s="66" t="s">
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="M2" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="W2" s="66" t="s">
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="W2" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="M3" s="63" t="s">
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="M3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="W3" s="63" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="72"/>
+      <c r="W3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
+      <c r="X3" s="72"/>
+      <c r="Y3" s="72"/>
+      <c r="Z3" s="72"/>
+      <c r="AA3" s="72"/>
+      <c r="AB3" s="72"/>
+      <c r="AC3" s="72"/>
+      <c r="AD3" s="72"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C4" s="38">
@@ -5316,7 +5336,7 @@
       <c r="J4" s="37">
         <v>32</v>
       </c>
-      <c r="K4" s="90"/>
+      <c r="K4" s="64"/>
       <c r="M4" s="38">
         <v>2</v>
       </c>
@@ -5367,7 +5387,7 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="37">
@@ -5455,7 +5475,7 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="37">
         <v>2</v>
       </c>
@@ -5541,7 +5561,7 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="37">
         <v>4</v>
       </c>
@@ -5627,7 +5647,7 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="37">
         <v>8</v>
       </c>
@@ -5713,7 +5733,7 @@
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="37">
         <v>16</v>
       </c>
@@ -5799,7 +5819,7 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="67"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="39">
         <v>32</v>
       </c>
@@ -5974,82 +5994,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
       <c r="L1" s="54"/>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
       <c r="V1" s="54"/>
-      <c r="W1" s="66" t="s">
+      <c r="W1" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="75"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="72" t="s">
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="74"/>
-      <c r="M2" s="72" t="s">
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
+      <c r="M2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="74"/>
-      <c r="W2" s="72" t="s">
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="83"/>
+      <c r="W2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="74"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="83"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C3" s="37">
@@ -6136,7 +6156,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="76" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="37">
@@ -6227,7 +6247,7 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
+      <c r="A5" s="77"/>
       <c r="B5" s="37">
         <v>4</v>
       </c>
@@ -6316,7 +6336,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="70"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="37">
         <v>6</v>
       </c>
@@ -6405,7 +6425,7 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="37">
         <v>8</v>
       </c>
@@ -6500,12 +6520,12 @@
       <c r="X8" s="35"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
       <c r="U9" s="35"/>
       <c r="V9" s="35"/>
       <c r="W9" s="35"/>
@@ -6671,53 +6691,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="I1" s="76" t="s">
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="I1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="O1" s="76" t="s">
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="O1" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="I2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="O2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C3" s="37">
@@ -6768,7 +6788,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="76" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="37">
@@ -6823,7 +6843,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
+      <c r="A5" s="77"/>
       <c r="B5" s="37">
         <v>4</v>
       </c>
@@ -6875,7 +6895,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="70"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="37">
         <v>6</v>
       </c>
@@ -6927,7 +6947,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="37">
         <v>8</v>
       </c>
@@ -7070,61 +7090,61 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
       <c r="H2" s="43"/>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="Q2" s="77" t="s">
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="Q2" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="87"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="74"/>
-      <c r="K3" s="63" t="s">
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="83"/>
+      <c r="K3" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
       <c r="P3" s="35"/>
-      <c r="S3" s="63" t="s">
+      <c r="S3" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="72"/>
+      <c r="W3" s="72"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C4" s="37">
@@ -7175,7 +7195,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="37">
@@ -7196,7 +7216,7 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="74" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="37">
@@ -7218,7 +7238,7 @@
         <v>0.56020000000000003</v>
       </c>
       <c r="P5" s="35"/>
-      <c r="Q5" s="67" t="s">
+      <c r="Q5" s="74" t="s">
         <v>18</v>
       </c>
       <c r="R5" s="37">
@@ -7241,7 +7261,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="37">
         <v>4</v>
       </c>
@@ -7260,7 +7280,7 @@
       <c r="G6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="67"/>
+      <c r="I6" s="74"/>
       <c r="J6" s="37">
         <v>4</v>
       </c>
@@ -7279,7 +7299,7 @@
       <c r="O6" s="2">
         <v>0.55220000000000002</v>
       </c>
-      <c r="Q6" s="67"/>
+      <c r="Q6" s="74"/>
       <c r="R6" s="37">
         <v>4</v>
       </c>
@@ -7300,7 +7320,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="37">
         <v>6</v>
       </c>
@@ -7319,7 +7339,7 @@
       <c r="G7" s="2">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I7" s="67"/>
+      <c r="I7" s="74"/>
       <c r="J7" s="37">
         <v>6</v>
       </c>
@@ -7338,7 +7358,7 @@
       <c r="O7" s="2">
         <v>0.55489999999999895</v>
       </c>
-      <c r="Q7" s="67"/>
+      <c r="Q7" s="74"/>
       <c r="R7" s="37">
         <v>6</v>
       </c>
@@ -7359,7 +7379,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="37">
         <v>8</v>
       </c>
@@ -7378,7 +7398,7 @@
       <c r="G8" s="2">
         <v>0.99975000000000003</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="37">
         <v>8</v>
       </c>
@@ -7397,7 +7417,7 @@
       <c r="O8" s="2">
         <v>0.55279999999999896</v>
       </c>
-      <c r="Q8" s="67"/>
+      <c r="Q8" s="74"/>
       <c r="R8" s="37">
         <v>8</v>
       </c>
@@ -7418,7 +7438,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="37">
         <v>10</v>
       </c>
@@ -7437,7 +7457,7 @@
       <c r="G9" s="2">
         <v>0.99929999999999897</v>
       </c>
-      <c r="I9" s="67"/>
+      <c r="I9" s="74"/>
       <c r="J9" s="37">
         <v>10</v>
       </c>
@@ -7456,7 +7476,7 @@
       <c r="O9" s="2">
         <v>0.55059999999999898</v>
       </c>
-      <c r="Q9" s="67"/>
+      <c r="Q9" s="74"/>
       <c r="R9" s="37">
         <v>10</v>
       </c>
@@ -7501,23 +7521,23 @@
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="86"/>
       <c r="J36" s="40"/>
       <c r="K36" s="40"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="95"/>
-      <c r="N36" s="95"/>
-      <c r="O36" s="95"/>
-      <c r="P36" s="95"/>
-      <c r="Q36" s="95"/>
-      <c r="R36" s="95"/>
-      <c r="S36" s="95"/>
+      <c r="M36" s="86"/>
+      <c r="N36" s="86"/>
+      <c r="O36" s="86"/>
+      <c r="P36" s="86"/>
+      <c r="Q36" s="86"/>
+      <c r="R36" s="86"/>
+      <c r="S36" s="86"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
@@ -7541,8 +7561,8 @@
       <c r="S37" s="41"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="96"/>
-      <c r="B38" s="90"/>
+      <c r="A38" s="85"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="36"/>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -7552,18 +7572,18 @@
       <c r="I38" s="36"/>
       <c r="J38" s="36"/>
       <c r="K38" s="36"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="97"/>
-      <c r="N38" s="97"/>
-      <c r="O38" s="97"/>
-      <c r="P38" s="97"/>
-      <c r="Q38" s="97"/>
-      <c r="R38" s="97"/>
-      <c r="S38" s="97"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="69"/>
+      <c r="S38" s="69"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="96"/>
-      <c r="B39" s="90"/>
+      <c r="A39" s="85"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="36"/>
       <c r="D39" s="36"/>
       <c r="E39" s="36"/>
@@ -7573,18 +7593,18 @@
       <c r="I39" s="36"/>
       <c r="J39" s="36"/>
       <c r="K39" s="36"/>
-      <c r="L39" s="90"/>
-      <c r="M39" s="97"/>
-      <c r="N39" s="97"/>
-      <c r="O39" s="97"/>
-      <c r="P39" s="97"/>
-      <c r="Q39" s="97"/>
-      <c r="R39" s="97"/>
-      <c r="S39" s="97"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="69"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="69"/>
+      <c r="S39" s="69"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="96"/>
-      <c r="B40" s="90"/>
+      <c r="A40" s="85"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="36"/>
       <c r="D40" s="36"/>
       <c r="E40" s="36"/>
@@ -7594,18 +7614,18 @@
       <c r="I40" s="36"/>
       <c r="J40" s="36"/>
       <c r="K40" s="36"/>
-      <c r="L40" s="90"/>
-      <c r="M40" s="97"/>
-      <c r="N40" s="97"/>
-      <c r="O40" s="97"/>
-      <c r="P40" s="97"/>
-      <c r="Q40" s="97"/>
-      <c r="R40" s="97"/>
-      <c r="S40" s="97"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="69"/>
+      <c r="R40" s="69"/>
+      <c r="S40" s="69"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="96"/>
-      <c r="B41" s="98"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="70"/>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
       <c r="E41" s="36"/>
@@ -7615,7 +7635,7 @@
       <c r="I41" s="36"/>
       <c r="J41" s="36"/>
       <c r="K41" s="36"/>
-      <c r="L41" s="98"/>
+      <c r="L41" s="70"/>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -7625,8 +7645,8 @@
       <c r="S41" s="5"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A42" s="96"/>
-      <c r="B42" s="98"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="70"/>
       <c r="C42" s="36"/>
       <c r="D42" s="36"/>
       <c r="E42" s="36"/>
@@ -7636,7 +7656,7 @@
       <c r="I42" s="36"/>
       <c r="J42" s="36"/>
       <c r="K42" s="36"/>
-      <c r="L42" s="98"/>
+      <c r="L42" s="70"/>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
@@ -7646,8 +7666,8 @@
       <c r="S42" s="5"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="96"/>
-      <c r="B43" s="90"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="64"/>
       <c r="C43" s="36"/>
       <c r="D43" s="36"/>
       <c r="E43" s="36"/>
@@ -7658,13 +7678,13 @@
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
       <c r="L43" s="5"/>
-      <c r="M43" s="97"/>
-      <c r="N43" s="97"/>
-      <c r="O43" s="97"/>
-      <c r="P43" s="97"/>
-      <c r="Q43" s="97"/>
-      <c r="R43" s="97"/>
-      <c r="S43" s="97"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="69"/>
+      <c r="P43" s="69"/>
+      <c r="Q43" s="69"/>
+      <c r="R43" s="69"/>
+      <c r="S43" s="69"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
@@ -7690,20 +7710,20 @@
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="95"/>
-      <c r="D45" s="95"/>
-      <c r="E45" s="95"/>
-      <c r="F45" s="95"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="95"/>
-      <c r="N45" s="95"/>
-      <c r="O45" s="95"/>
-      <c r="P45" s="95"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="86"/>
+      <c r="P45" s="86"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
@@ -7711,27 +7731,27 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="90"/>
-      <c r="N46" s="90"/>
-      <c r="O46" s="90"/>
-      <c r="P46" s="90"/>
+      <c r="M46" s="64"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="64"/>
+      <c r="P46" s="64"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A47" s="96"/>
-      <c r="B47" s="90"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="36"/>
       <c r="D47" s="36"/>
       <c r="E47" s="36"/>
@@ -7741,7 +7761,7 @@
       <c r="I47" s="36"/>
       <c r="J47" s="36"/>
       <c r="K47" s="36"/>
-      <c r="L47" s="90"/>
+      <c r="L47" s="64"/>
       <c r="M47" s="36"/>
       <c r="N47" s="36"/>
       <c r="O47" s="36"/>
@@ -7751,8 +7771,8 @@
       <c r="S47" s="5"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A48" s="96"/>
-      <c r="B48" s="90"/>
+      <c r="A48" s="85"/>
+      <c r="B48" s="64"/>
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
       <c r="E48" s="36"/>
@@ -7762,7 +7782,7 @@
       <c r="I48" s="36"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
-      <c r="L48" s="90"/>
+      <c r="L48" s="64"/>
       <c r="M48" s="36"/>
       <c r="N48" s="36"/>
       <c r="O48" s="36"/>
@@ -7772,8 +7792,8 @@
       <c r="S48" s="5"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="96"/>
-      <c r="B49" s="90"/>
+      <c r="A49" s="85"/>
+      <c r="B49" s="64"/>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
       <c r="E49" s="36"/>
@@ -7783,7 +7803,7 @@
       <c r="I49" s="36"/>
       <c r="J49" s="36"/>
       <c r="K49" s="36"/>
-      <c r="L49" s="90"/>
+      <c r="L49" s="64"/>
       <c r="M49" s="36"/>
       <c r="N49" s="36"/>
       <c r="O49" s="36"/>
@@ -7793,8 +7813,8 @@
       <c r="S49" s="5"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="96"/>
-      <c r="B50" s="90"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="64"/>
       <c r="C50" s="36"/>
       <c r="D50" s="36"/>
       <c r="E50" s="36"/>
@@ -7804,7 +7824,7 @@
       <c r="I50" s="36"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="90"/>
+      <c r="L50" s="64"/>
       <c r="M50" s="36"/>
       <c r="N50" s="36"/>
       <c r="O50" s="36"/>
@@ -7838,47 +7858,47 @@
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="95"/>
-      <c r="F52" s="95"/>
-      <c r="G52" s="95"/>
-      <c r="H52" s="95"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
+      <c r="H52" s="86"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
-      <c r="N52" s="95"/>
-      <c r="O52" s="95"/>
-      <c r="P52" s="95"/>
-      <c r="Q52" s="95"/>
-      <c r="R52" s="95"/>
+      <c r="N52" s="86"/>
+      <c r="O52" s="86"/>
+      <c r="P52" s="86"/>
+      <c r="Q52" s="86"/>
+      <c r="R52" s="86"/>
       <c r="S52" s="5"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90"/>
-      <c r="E53" s="90"/>
-      <c r="F53" s="90"/>
-      <c r="G53" s="98"/>
-      <c r="H53" s="98"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
-      <c r="M53" s="90"/>
-      <c r="N53" s="90"/>
-      <c r="O53" s="90"/>
-      <c r="P53" s="90"/>
-      <c r="Q53" s="98"/>
-      <c r="R53" s="98"/>
+      <c r="M53" s="64"/>
+      <c r="N53" s="64"/>
+      <c r="O53" s="64"/>
+      <c r="P53" s="64"/>
+      <c r="Q53" s="70"/>
+      <c r="R53" s="70"/>
       <c r="S53" s="5"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A54" s="96"/>
-      <c r="B54" s="90"/>
+      <c r="A54" s="85"/>
+      <c r="B54" s="64"/>
       <c r="C54" s="36"/>
       <c r="D54" s="36"/>
       <c r="E54" s="36"/>
@@ -7888,18 +7908,18 @@
       <c r="I54" s="36"/>
       <c r="J54" s="36"/>
       <c r="K54" s="36"/>
-      <c r="L54" s="90"/>
+      <c r="L54" s="64"/>
       <c r="M54" s="36"/>
-      <c r="N54" s="97"/>
-      <c r="O54" s="97"/>
-      <c r="P54" s="97"/>
-      <c r="Q54" s="97"/>
-      <c r="R54" s="97"/>
+      <c r="N54" s="69"/>
+      <c r="O54" s="69"/>
+      <c r="P54" s="69"/>
+      <c r="Q54" s="69"/>
+      <c r="R54" s="69"/>
       <c r="S54" s="5"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A55" s="96"/>
-      <c r="B55" s="90"/>
+      <c r="A55" s="85"/>
+      <c r="B55" s="64"/>
       <c r="C55" s="36"/>
       <c r="D55" s="36"/>
       <c r="E55" s="36"/>
@@ -7909,18 +7929,18 @@
       <c r="I55" s="36"/>
       <c r="J55" s="36"/>
       <c r="K55" s="36"/>
-      <c r="L55" s="90"/>
+      <c r="L55" s="64"/>
       <c r="M55" s="36"/>
-      <c r="N55" s="97"/>
-      <c r="O55" s="97"/>
-      <c r="P55" s="97"/>
-      <c r="Q55" s="97"/>
-      <c r="R55" s="97"/>
+      <c r="N55" s="69"/>
+      <c r="O55" s="69"/>
+      <c r="P55" s="69"/>
+      <c r="Q55" s="69"/>
+      <c r="R55" s="69"/>
       <c r="S55" s="5"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A56" s="96"/>
-      <c r="B56" s="90"/>
+      <c r="A56" s="85"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="36"/>
       <c r="D56" s="36"/>
       <c r="E56" s="36"/>
@@ -7930,18 +7950,18 @@
       <c r="I56" s="36"/>
       <c r="J56" s="36"/>
       <c r="K56" s="36"/>
-      <c r="L56" s="90"/>
+      <c r="L56" s="64"/>
       <c r="M56" s="36"/>
-      <c r="N56" s="97"/>
-      <c r="O56" s="97"/>
-      <c r="P56" s="97"/>
-      <c r="Q56" s="97"/>
-      <c r="R56" s="97"/>
+      <c r="N56" s="69"/>
+      <c r="O56" s="69"/>
+      <c r="P56" s="69"/>
+      <c r="Q56" s="69"/>
+      <c r="R56" s="69"/>
       <c r="S56" s="5"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A57" s="96"/>
-      <c r="B57" s="90"/>
+      <c r="A57" s="85"/>
+      <c r="B57" s="64"/>
       <c r="C57" s="36"/>
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
@@ -7951,17 +7971,26 @@
       <c r="I57" s="36"/>
       <c r="J57" s="36"/>
       <c r="K57" s="36"/>
-      <c r="L57" s="90"/>
+      <c r="L57" s="64"/>
       <c r="M57" s="36"/>
-      <c r="N57" s="97"/>
-      <c r="O57" s="97"/>
-      <c r="P57" s="97"/>
-      <c r="Q57" s="97"/>
-      <c r="R57" s="97"/>
+      <c r="N57" s="69"/>
+      <c r="O57" s="69"/>
+      <c r="P57" s="69"/>
+      <c r="Q57" s="69"/>
+      <c r="R57" s="69"/>
       <c r="S57" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="Q5:Q9"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="I5:I9"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="N52:R52"/>
     <mergeCell ref="D52:H52"/>
@@ -7971,15 +8000,6 @@
     <mergeCell ref="C45:F45"/>
     <mergeCell ref="M45:P45"/>
     <mergeCell ref="A47:A50"/>
-    <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="S3:W3"/>
-    <mergeCell ref="Q5:Q9"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="I5:I9"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="I2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="P3:P5">
     <cfRule type="colorScale" priority="9">
@@ -8111,7 +8131,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8136,54 +8156,54 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="I2" s="78" t="s">
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="I2" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="P2" s="78" t="s">
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="P2" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="J3" s="63" t="s">
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="J3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="Q3" s="63" t="s">
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="Q3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C4" s="38">
@@ -8233,7 +8253,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="76" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="37">
@@ -8292,7 +8312,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="70"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="37">
         <v>28</v>
       </c>
@@ -8349,7 +8369,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="70"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="37">
         <v>32</v>
       </c>
@@ -8406,7 +8426,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="70"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="37">
         <v>40</v>
       </c>
@@ -8463,7 +8483,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="37">
         <v>48</v>
       </c>
@@ -8520,7 +8540,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="70"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="39">
         <v>64</v>
       </c>
@@ -8579,7 +8599,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="71"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="39">
         <v>128</v>
       </c>
@@ -8760,45 +8780,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="K1" s="76" t="s">
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="K1" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="63" t="s">
+      <c r="K2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C3" s="37">
@@ -8846,7 +8866,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="74" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="37">
@@ -8896,7 +8916,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="37">
         <v>100</v>
       </c>
@@ -8944,7 +8964,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="37">
         <v>200</v>
       </c>
@@ -8992,7 +9012,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="37">
         <v>500</v>
       </c>
@@ -9040,7 +9060,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="37">
         <v>1000</v>
       </c>
@@ -9088,7 +9108,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="37">
         <v>2000</v>
       </c>

</xml_diff>